<commit_message>
Updating daily stats for July 3
</commit_message>
<xml_diff>
--- a/assets/My_Hitter_Listing.xlsx
+++ b/assets/My_Hitter_Listing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Python\dash\dashenv\github\matchup\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{710B9E37-F68C-416B-A0BD-F43B0347C3B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E18C8714-A46E-4533-BAB5-47259A5EEA7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -10459,9 +10459,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:M1770"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1746" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1770" sqref="E1770"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A734" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K748" sqref="K748"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -24400,7 +24400,7 @@
         <v>3126</v>
       </c>
       <c r="M358" t="s">
-        <v>844</v>
+        <v>3126</v>
       </c>
     </row>
     <row r="359" spans="1:13" x14ac:dyDescent="0.3">
@@ -39357,10 +39357,10 @@
         <v>128</v>
       </c>
       <c r="B747" t="s">
-        <v>1428</v>
+        <v>1409</v>
       </c>
       <c r="C747" t="s">
-        <v>1458</v>
+        <v>1438</v>
       </c>
       <c r="D747" t="s">
         <v>1463</v>
@@ -39382,6 +39382,9 @@
       </c>
       <c r="J747" t="s">
         <v>128</v>
+      </c>
+      <c r="K747">
+        <v>642851</v>
       </c>
       <c r="L747" t="s">
         <v>128</v>

</xml_diff>

<commit_message>
Updating daily stats for July 4
</commit_message>
<xml_diff>
--- a/assets/My_Hitter_Listing.xlsx
+++ b/assets/My_Hitter_Listing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Python\dash\dashenv\github\matchup\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C224B21A-5648-4F62-8E27-CC9DF1477B93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9377C989-3039-44A2-9DEC-ACA3406086E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20719" uniqueCount="3347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20730" uniqueCount="3348">
   <si>
     <t>mlb_name</t>
   </si>
@@ -10073,7 +10073,10 @@
     <t>Brooks Lee</t>
   </si>
   <si>
-    <t>sa3019973</t>
+    <t>Leo Jimenez</t>
+  </si>
+  <si>
+    <t>sa3006891</t>
   </si>
 </sst>
 </file>
@@ -10463,11 +10466,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:M1771"/>
+  <dimension ref="A1:M1772"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1747" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G1771" sqref="G1771"/>
+      <pane ySplit="1" topLeftCell="A1748" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E1772" sqref="E1772"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -79280,14 +79283,14 @@
       <c r="D1771" t="s">
         <v>1465</v>
       </c>
-      <c r="E1771" t="s">
-        <v>3346</v>
+      <c r="E1771">
+        <v>31595</v>
       </c>
       <c r="F1771" t="s">
         <v>3345</v>
       </c>
       <c r="G1771" t="s">
-        <v>1399</v>
+        <v>1400</v>
       </c>
       <c r="H1771" t="s">
         <v>3345</v>
@@ -79303,6 +79306,44 @@
       </c>
       <c r="M1771" t="s">
         <v>3345</v>
+      </c>
+    </row>
+    <row r="1772" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1772" t="s">
+        <v>3346</v>
+      </c>
+      <c r="B1772" t="s">
+        <v>1429</v>
+      </c>
+      <c r="C1772" t="s">
+        <v>1459</v>
+      </c>
+      <c r="D1772" t="s">
+        <v>1463</v>
+      </c>
+      <c r="E1772" t="s">
+        <v>3347</v>
+      </c>
+      <c r="F1772" t="s">
+        <v>3346</v>
+      </c>
+      <c r="G1772" t="s">
+        <v>2806</v>
+      </c>
+      <c r="H1772" t="s">
+        <v>3346</v>
+      </c>
+      <c r="I1772" t="s">
+        <v>3346</v>
+      </c>
+      <c r="J1772" t="s">
+        <v>3346</v>
+      </c>
+      <c r="L1772" t="s">
+        <v>3346</v>
+      </c>
+      <c r="M1772" t="s">
+        <v>3346</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating daily stats for July 6
</commit_message>
<xml_diff>
--- a/assets/My_Hitter_Listing.xlsx
+++ b/assets/My_Hitter_Listing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Python\dash\dashenv\github\matchup\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9377C989-3039-44A2-9DEC-ACA3406086E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3C0D5F8-FF83-44A5-B69A-6EF8627F791A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20730" uniqueCount="3348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20729" uniqueCount="3347">
   <si>
     <t>mlb_name</t>
   </si>
@@ -10074,9 +10074,6 @@
   </si>
   <si>
     <t>Leo Jimenez</t>
-  </si>
-  <si>
-    <t>sa3006891</t>
   </si>
 </sst>
 </file>
@@ -10469,8 +10466,8 @@
   <dimension ref="A1:M1772"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1748" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1772" sqref="E1772"/>
+      <pane ySplit="1" topLeftCell="A1763" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E1773" sqref="E1773"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -57508,10 +57505,10 @@
         <v>808</v>
       </c>
       <c r="B1217" t="s">
-        <v>1425</v>
+        <v>1404</v>
       </c>
       <c r="C1217" t="s">
-        <v>1455</v>
+        <v>1433</v>
       </c>
       <c r="D1217" t="s">
         <v>1463</v>
@@ -70580,7 +70577,7 @@
         <v>3057</v>
       </c>
       <c r="M1553" t="s">
-        <v>3053</v>
+        <v>3057</v>
       </c>
     </row>
     <row r="1554" spans="1:13" x14ac:dyDescent="0.3">
@@ -72183,10 +72180,10 @@
         <v>3099</v>
       </c>
       <c r="B1594" t="s">
-        <v>1427</v>
+        <v>3220</v>
       </c>
       <c r="C1594" t="s">
-        <v>1457</v>
+        <v>1443</v>
       </c>
       <c r="D1594" t="s">
         <v>1463</v>
@@ -79321,14 +79318,14 @@
       <c r="D1772" t="s">
         <v>1463</v>
       </c>
-      <c r="E1772" t="s">
-        <v>3347</v>
+      <c r="E1772">
+        <v>23782</v>
       </c>
       <c r="F1772" t="s">
         <v>3346</v>
       </c>
       <c r="G1772" t="s">
-        <v>2806</v>
+        <v>1399</v>
       </c>
       <c r="H1772" t="s">
         <v>3346</v>

</xml_diff>

<commit_message>
Updating daily stats for July 7
</commit_message>
<xml_diff>
--- a/assets/My_Hitter_Listing.xlsx
+++ b/assets/My_Hitter_Listing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Python\dash\dashenv\github\matchup\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3C0D5F8-FF83-44A5-B69A-6EF8627F791A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{455000D6-B7D0-428C-B1F4-0DC3DB33F157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20729" uniqueCount="3347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20740" uniqueCount="3348">
   <si>
     <t>mlb_name</t>
   </si>
@@ -10074,6 +10074,9 @@
   </si>
   <si>
     <t>Leo Jimenez</t>
+  </si>
+  <si>
+    <t>Vinny Capra</t>
   </si>
 </sst>
 </file>
@@ -10463,11 +10466,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:M1772"/>
+  <dimension ref="A1:M1773"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A1763" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1773" sqref="E1773"/>
+      <selection pane="bottomLeft" activeCell="E1774" sqref="E1774"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -79343,6 +79346,44 @@
         <v>3346</v>
       </c>
     </row>
+    <row r="1773" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1773" t="s">
+        <v>3347</v>
+      </c>
+      <c r="B1773" t="s">
+        <v>1425</v>
+      </c>
+      <c r="C1773" t="s">
+        <v>1455</v>
+      </c>
+      <c r="D1773" t="s">
+        <v>1463</v>
+      </c>
+      <c r="E1773">
+        <v>25040</v>
+      </c>
+      <c r="F1773" t="s">
+        <v>3347</v>
+      </c>
+      <c r="G1773" t="s">
+        <v>2810</v>
+      </c>
+      <c r="H1773" t="s">
+        <v>3347</v>
+      </c>
+      <c r="I1773" t="s">
+        <v>3347</v>
+      </c>
+      <c r="J1773" t="s">
+        <v>3347</v>
+      </c>
+      <c r="L1773" t="s">
+        <v>3347</v>
+      </c>
+      <c r="M1773" t="s">
+        <v>3347</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I1395">
     <sortCondition ref="A2:A1395"/>

</xml_diff>

<commit_message>
Updating daily stats for July 8
</commit_message>
<xml_diff>
--- a/assets/My_Hitter_Listing.xlsx
+++ b/assets/My_Hitter_Listing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Python\dash\dashenv\github\matchup\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{455000D6-B7D0-428C-B1F4-0DC3DB33F157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE152378-3212-4027-A925-A0E653C8C7C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20740" uniqueCount="3348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20740" uniqueCount="3349">
   <si>
     <t>mlb_name</t>
   </si>
@@ -10077,6 +10077,9 @@
   </si>
   <si>
     <t>Vinny Capra</t>
+  </si>
+  <si>
+    <t>Edwin Ríos</t>
   </si>
 </sst>
 </file>
@@ -10468,9 +10471,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:M1773"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1763" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1774" sqref="E1774"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1331" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M1344" sqref="M1344"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -62391,10 +62394,10 @@
         <v>446</v>
       </c>
       <c r="B1344" t="s">
-        <v>1417</v>
+        <v>1409</v>
       </c>
       <c r="C1344" t="s">
-        <v>1447</v>
+        <v>1438</v>
       </c>
       <c r="D1344" t="s">
         <v>1464</v>
@@ -62415,10 +62418,13 @@
         <v>446</v>
       </c>
       <c r="J1344" t="s">
-        <v>446</v>
+        <v>3348</v>
+      </c>
+      <c r="K1344">
+        <v>621458</v>
       </c>
       <c r="L1344" t="s">
-        <v>446</v>
+        <v>3348</v>
       </c>
       <c r="M1344" t="s">
         <v>446</v>

</xml_diff>

<commit_message>
Updating daily files for July 12
</commit_message>
<xml_diff>
--- a/assets/My_Hitter_Listing.xlsx
+++ b/assets/My_Hitter_Listing.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27820"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27830"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Python\dash\dashenv\github\matchup\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62D30387-F328-4BE1-B3F4-7B02AAB8E5F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B44A4B6-95F3-461E-BD0D-32E43A3B00A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -10471,9 +10471,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:M1774"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1750" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1755" sqref="E1755"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A127" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J140" sqref="J140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11518,7 +11518,7 @@
         <v>1327</v>
       </c>
       <c r="J26" t="s">
-        <v>1327</v>
+        <v>3170</v>
       </c>
       <c r="K26">
         <v>660644</v>
@@ -15960,7 +15960,7 @@
         <v>667</v>
       </c>
       <c r="J140" t="s">
-        <v>667</v>
+        <v>3169</v>
       </c>
       <c r="K140">
         <v>660821</v>

</xml_diff>

<commit_message>
Updating daily files July 20
</commit_message>
<xml_diff>
--- a/assets/My_Hitter_Listing.xlsx
+++ b/assets/My_Hitter_Listing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Python\dash\dashenv\github\matchup\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07F2D57A-3865-4F92-89A9-FF7DA79A19B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5D35F26-A16B-4CE8-9710-3190E7F13D4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4008" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Players" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20773" uniqueCount="3353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20783" uniqueCount="3353">
   <si>
     <t>mlb_name</t>
   </si>
@@ -10088,10 +10088,10 @@
     <t>Brooks Baldwin</t>
   </si>
   <si>
-    <t>sa3019918</t>
-  </si>
-  <si>
     <t>Riley Baldwin</t>
+  </si>
+  <si>
+    <t>Chuckie Robinson</t>
   </si>
 </sst>
 </file>
@@ -10481,11 +10481,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:M1776"/>
+  <dimension ref="A1:M1777"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A1764" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1777" sqref="F1777"/>
+      <selection pane="bottomLeft" activeCell="E1777" sqref="E1777"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -79491,14 +79491,14 @@
       <c r="D1776" t="s">
         <v>1465</v>
       </c>
-      <c r="E1776" t="s">
+      <c r="E1776">
+        <v>31394</v>
+      </c>
+      <c r="F1776" t="s">
         <v>3351</v>
       </c>
-      <c r="F1776" t="s">
-        <v>3352</v>
-      </c>
       <c r="G1776" t="s">
-        <v>2815</v>
+        <v>1401</v>
       </c>
       <c r="H1776" t="s">
         <v>3350</v>
@@ -79514,6 +79514,44 @@
       </c>
       <c r="M1776" t="s">
         <v>3350</v>
+      </c>
+    </row>
+    <row r="1777" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1777" t="s">
+        <v>3352</v>
+      </c>
+      <c r="B1777" t="s">
+        <v>1415</v>
+      </c>
+      <c r="C1777" t="s">
+        <v>1445</v>
+      </c>
+      <c r="D1777" t="s">
+        <v>1463</v>
+      </c>
+      <c r="E1777">
+        <v>19824</v>
+      </c>
+      <c r="F1777" t="s">
+        <v>3352</v>
+      </c>
+      <c r="G1777" t="s">
+        <v>1397</v>
+      </c>
+      <c r="H1777" t="s">
+        <v>3352</v>
+      </c>
+      <c r="I1777" t="s">
+        <v>3352</v>
+      </c>
+      <c r="J1777" t="s">
+        <v>3352</v>
+      </c>
+      <c r="L1777" t="s">
+        <v>3352</v>
+      </c>
+      <c r="M1777" t="s">
+        <v>3352</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating daily files July 21
</commit_message>
<xml_diff>
--- a/assets/My_Hitter_Listing.xlsx
+++ b/assets/My_Hitter_Listing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Python\dash\dashenv\github\matchup\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5D35F26-A16B-4CE8-9710-3190E7F13D4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C30AC412-A81C-4B82-8E48-14D17104DF7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -10483,9 +10483,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:M1777"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1764" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1777" sqref="E1777"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1629" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O1642" sqref="O1642"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -74112,10 +74112,10 @@
         <v>3193</v>
       </c>
       <c r="B1642" t="s">
-        <v>1422</v>
+        <v>1430</v>
       </c>
       <c r="C1642" t="s">
-        <v>1452</v>
+        <v>1460</v>
       </c>
       <c r="D1642" t="s">
         <v>1464</v>

</xml_diff>

<commit_message>
Updating daily files July 22
</commit_message>
<xml_diff>
--- a/assets/My_Hitter_Listing.xlsx
+++ b/assets/My_Hitter_Listing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Python\dash\dashenv\github\matchup\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C30AC412-A81C-4B82-8E48-14D17104DF7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB49D0C6-AF18-4751-8DE1-5F831EEA9129}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20783" uniqueCount="3353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20795" uniqueCount="3357">
   <si>
     <t>mlb_name</t>
   </si>
@@ -10092,6 +10092,18 @@
   </si>
   <si>
     <t>Chuckie Robinson</t>
+  </si>
+  <si>
+    <t>Nacho Alvarez</t>
+  </si>
+  <si>
+    <t>Ignacio Alvarez</t>
+  </si>
+  <si>
+    <t>sa3019905</t>
+  </si>
+  <si>
+    <t>Diego A. Castillo</t>
   </si>
 </sst>
 </file>
@@ -10481,11 +10493,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:M1777"/>
+  <dimension ref="A1:M1778"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1629" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O1642" sqref="O1642"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1489" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G1502" sqref="G1502"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -68525,7 +68537,7 @@
         <v>1400</v>
       </c>
       <c r="H1502" t="s">
-        <v>2999</v>
+        <v>3356</v>
       </c>
       <c r="I1502" t="s">
         <v>2999</v>
@@ -79552,6 +79564,47 @@
       </c>
       <c r="M1777" t="s">
         <v>3352</v>
+      </c>
+    </row>
+    <row r="1778" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1778" t="s">
+        <v>3353</v>
+      </c>
+      <c r="B1778" t="s">
+        <v>1408</v>
+      </c>
+      <c r="C1778" t="s">
+        <v>1437</v>
+      </c>
+      <c r="D1778" t="s">
+        <v>1463</v>
+      </c>
+      <c r="E1778" t="s">
+        <v>3355</v>
+      </c>
+      <c r="F1778" t="s">
+        <v>3354</v>
+      </c>
+      <c r="G1778" t="s">
+        <v>1399</v>
+      </c>
+      <c r="H1778" t="s">
+        <v>3353</v>
+      </c>
+      <c r="I1778" t="s">
+        <v>3353</v>
+      </c>
+      <c r="J1778" t="s">
+        <v>3353</v>
+      </c>
+      <c r="K1778">
+        <v>805373</v>
+      </c>
+      <c r="L1778" t="s">
+        <v>3353</v>
+      </c>
+      <c r="M1778" t="s">
+        <v>3353</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating daily files July 23
</commit_message>
<xml_diff>
--- a/assets/My_Hitter_Listing.xlsx
+++ b/assets/My_Hitter_Listing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Python\dash\dashenv\github\matchup\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB49D0C6-AF18-4751-8DE1-5F831EEA9129}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C582F08-B567-458C-AF27-EDA7A91F1BCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20795" uniqueCount="3357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20806" uniqueCount="3358">
   <si>
     <t>mlb_name</t>
   </si>
@@ -10100,10 +10100,13 @@
     <t>Ignacio Alvarez</t>
   </si>
   <si>
-    <t>sa3019905</t>
-  </si>
-  <si>
     <t>Diego A. Castillo</t>
+  </si>
+  <si>
+    <t>Carlos Narvaez</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -10493,11 +10496,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:M1778"/>
+  <dimension ref="A1:M1779"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1489" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G1502" sqref="G1502"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1755" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K1780" sqref="K1780"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -49569,10 +49572,10 @@
         <v>2904</v>
       </c>
       <c r="B1011" t="s">
-        <v>1409</v>
+        <v>1432</v>
       </c>
       <c r="C1011" t="s">
-        <v>1438</v>
+        <v>1462</v>
       </c>
       <c r="D1011" t="s">
         <v>1464</v>
@@ -49594,6 +49597,9 @@
       </c>
       <c r="J1011" t="s">
         <v>2904</v>
+      </c>
+      <c r="K1011" t="s">
+        <v>3357</v>
       </c>
       <c r="L1011" t="s">
         <v>2904</v>
@@ -68537,7 +68543,7 @@
         <v>1400</v>
       </c>
       <c r="H1502" t="s">
-        <v>3356</v>
+        <v>3355</v>
       </c>
       <c r="I1502" t="s">
         <v>2999</v>
@@ -79579,14 +79585,14 @@
       <c r="D1778" t="s">
         <v>1463</v>
       </c>
-      <c r="E1778" t="s">
-        <v>3355</v>
+      <c r="E1778">
+        <v>31765</v>
       </c>
       <c r="F1778" t="s">
         <v>3354</v>
       </c>
       <c r="G1778" t="s">
-        <v>1399</v>
+        <v>1401</v>
       </c>
       <c r="H1778" t="s">
         <v>3353</v>
@@ -79605,6 +79611,47 @@
       </c>
       <c r="M1778" t="s">
         <v>3353</v>
+      </c>
+    </row>
+    <row r="1779" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1779" t="s">
+        <v>3356</v>
+      </c>
+      <c r="B1779" t="s">
+        <v>1419</v>
+      </c>
+      <c r="C1779" t="s">
+        <v>1449</v>
+      </c>
+      <c r="D1779" t="s">
+        <v>1463</v>
+      </c>
+      <c r="E1779">
+        <v>19722</v>
+      </c>
+      <c r="F1779" t="s">
+        <v>3356</v>
+      </c>
+      <c r="G1779" t="s">
+        <v>1397</v>
+      </c>
+      <c r="H1779" t="s">
+        <v>3356</v>
+      </c>
+      <c r="I1779" t="s">
+        <v>3356</v>
+      </c>
+      <c r="J1779" t="s">
+        <v>3356</v>
+      </c>
+      <c r="K1779">
+        <v>665966</v>
+      </c>
+      <c r="L1779" t="s">
+        <v>3356</v>
+      </c>
+      <c r="M1779" t="s">
+        <v>3356</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating daily files July 25
</commit_message>
<xml_diff>
--- a/assets/My_Hitter_Listing.xlsx
+++ b/assets/My_Hitter_Listing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Python\dash\dashenv\github\matchup\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C582F08-B567-458C-AF27-EDA7A91F1BCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{511D3AC6-4790-4C68-A18A-33F1B859D66A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -10499,8 +10499,8 @@
   <dimension ref="A1:M1779"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1755" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K1780" sqref="K1780"/>
+      <pane ySplit="1" topLeftCell="A601" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M614" sqref="M614"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -34228,10 +34228,10 @@
         <v>395</v>
       </c>
       <c r="B614" t="s">
-        <v>1407</v>
+        <v>1420</v>
       </c>
       <c r="C614" t="s">
-        <v>1436</v>
+        <v>1450</v>
       </c>
       <c r="D614" t="s">
         <v>1463</v>

</xml_diff>

<commit_message>
Updating daily files July 26
</commit_message>
<xml_diff>
--- a/assets/My_Hitter_Listing.xlsx
+++ b/assets/My_Hitter_Listing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Python\dash\dashenv\github\matchup\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{511D3AC6-4790-4C68-A18A-33F1B859D66A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C582E31-36BE-4679-9C29-04CA2F0BCA8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -10498,9 +10498,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:M1779"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A601" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M614" sqref="M614"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A364" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B378" sqref="B378"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12498,10 +12498,10 @@
         <v>1013</v>
       </c>
       <c r="B51" t="s">
-        <v>1420</v>
+        <v>1410</v>
       </c>
       <c r="C51" t="s">
-        <v>1450</v>
+        <v>1439</v>
       </c>
       <c r="D51" t="s">
         <v>1463</v>
@@ -25155,10 +25155,10 @@
         <v>1094</v>
       </c>
       <c r="B377" t="s">
-        <v>1423</v>
+        <v>1432</v>
       </c>
       <c r="C377" t="s">
-        <v>1453</v>
+        <v>1462</v>
       </c>
       <c r="D377" t="s">
         <v>1463</v>

</xml_diff>

<commit_message>
Updating daily files July 28
</commit_message>
<xml_diff>
--- a/assets/My_Hitter_Listing.xlsx
+++ b/assets/My_Hitter_Listing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Python\dash\dashenv\github\matchup\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E004866-70A8-417B-BE25-93B9858264AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86D21ADD-BC67-4368-87DE-AE1AE6BAFF42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20760" uniqueCount="3313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20771" uniqueCount="3314">
   <si>
     <t>mlb_name</t>
   </si>
@@ -9972,6 +9972,9 @@
   </si>
   <si>
     <t>Benjamin Rice</t>
+  </si>
+  <si>
+    <t>Leo Rivas</t>
   </si>
 </sst>
 </file>
@@ -10047,7 +10050,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -10056,7 +10059,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -10362,11 +10364,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:M1779"/>
+  <dimension ref="A1:M1780"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1386" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1390" sqref="E1390"/>
+      <pane ySplit="1" topLeftCell="A1756" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1780" sqref="A1780"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -25182,10 +25184,10 @@
         <v>119</v>
       </c>
       <c r="B381" t="s">
-        <v>1414</v>
+        <v>1418</v>
       </c>
       <c r="C381" t="s">
-        <v>1444</v>
+        <v>1448</v>
       </c>
       <c r="D381" t="s">
         <v>1463</v>
@@ -36849,10 +36851,10 @@
         <v>291</v>
       </c>
       <c r="B685" t="s">
-        <v>1416</v>
+        <v>1417</v>
       </c>
       <c r="C685" t="s">
-        <v>1446</v>
+        <v>1447</v>
       </c>
       <c r="D685" t="s">
         <v>1463</v>
@@ -51757,10 +51759,10 @@
         <v>641</v>
       </c>
       <c r="B1071" t="s">
-        <v>1416</v>
+        <v>1419</v>
       </c>
       <c r="C1071" t="s">
-        <v>1446</v>
+        <v>1449</v>
       </c>
       <c r="D1071" t="s">
         <v>1464</v>
@@ -51782,6 +51784,9 @@
       </c>
       <c r="J1071" t="s">
         <v>2892</v>
+      </c>
+      <c r="K1071">
+        <v>665862</v>
       </c>
       <c r="L1071" t="s">
         <v>2892</v>
@@ -63064,7 +63069,7 @@
       <c r="D1364" t="s">
         <v>1464</v>
       </c>
-      <c r="E1364" s="4">
+      <c r="E1364">
         <v>13301</v>
       </c>
       <c r="F1364" t="s">
@@ -63105,7 +63110,7 @@
       <c r="D1365" t="s">
         <v>1463</v>
       </c>
-      <c r="E1365" s="4">
+      <c r="E1365">
         <v>17321</v>
       </c>
       <c r="F1365" t="s">
@@ -63146,7 +63151,7 @@
       <c r="D1366" t="s">
         <v>1463</v>
       </c>
-      <c r="E1366" s="4">
+      <c r="E1366">
         <v>2073</v>
       </c>
       <c r="F1366" t="s">
@@ -63184,7 +63189,7 @@
       <c r="D1367" t="s">
         <v>1464</v>
       </c>
-      <c r="E1367" s="4">
+      <c r="E1367">
         <v>4316</v>
       </c>
       <c r="F1367" t="s">
@@ -63222,7 +63227,7 @@
       <c r="D1368" t="s">
         <v>1463</v>
       </c>
-      <c r="E1368" s="4">
+      <c r="E1368">
         <v>4898</v>
       </c>
       <c r="F1368" t="s">
@@ -63260,7 +63265,7 @@
       <c r="D1369" t="s">
         <v>1464</v>
       </c>
-      <c r="E1369" s="4">
+      <c r="E1369">
         <v>10264</v>
       </c>
       <c r="F1369" t="s">
@@ -63301,7 +63306,7 @@
       <c r="D1370" t="s">
         <v>1463</v>
       </c>
-      <c r="E1370" s="4">
+      <c r="E1370">
         <v>10349</v>
       </c>
       <c r="F1370" t="s">
@@ -63380,7 +63385,7 @@
       <c r="D1372" t="s">
         <v>1463</v>
       </c>
-      <c r="E1372" s="4">
+      <c r="E1372">
         <v>11147</v>
       </c>
       <c r="F1372" t="s">
@@ -63418,7 +63423,7 @@
       <c r="D1373" t="s">
         <v>1464</v>
       </c>
-      <c r="E1373" s="4">
+      <c r="E1373">
         <v>11251</v>
       </c>
       <c r="F1373" t="s">
@@ -63456,7 +63461,7 @@
       <c r="D1374" t="s">
         <v>1463</v>
       </c>
-      <c r="E1374" s="4">
+      <c r="E1374">
         <v>11342</v>
       </c>
       <c r="F1374" t="s">
@@ -63494,7 +63499,7 @@
       <c r="D1375" t="s">
         <v>1463</v>
       </c>
-      <c r="E1375" s="4">
+      <c r="E1375">
         <v>1177</v>
       </c>
       <c r="F1375" t="s">
@@ -63532,7 +63537,7 @@
       <c r="D1376" t="s">
         <v>1463</v>
       </c>
-      <c r="E1376" s="4">
+      <c r="E1376">
         <v>11773</v>
       </c>
       <c r="F1376" t="s">
@@ -63570,7 +63575,7 @@
       <c r="D1377" t="s">
         <v>1463</v>
       </c>
-      <c r="E1377" s="4">
+      <c r="E1377">
         <v>11850</v>
       </c>
       <c r="F1377" t="s">
@@ -63608,7 +63613,7 @@
       <c r="D1378" t="s">
         <v>1464</v>
       </c>
-      <c r="E1378" s="4">
+      <c r="E1378">
         <v>12244</v>
       </c>
       <c r="F1378" t="s">
@@ -63646,7 +63651,7 @@
       <c r="D1379" t="s">
         <v>1465</v>
       </c>
-      <c r="E1379" s="4">
+      <c r="E1379">
         <v>1281</v>
       </c>
       <c r="F1379" t="s">
@@ -63684,7 +63689,7 @@
       <c r="D1380" t="s">
         <v>1465</v>
       </c>
-      <c r="E1380" s="4">
+      <c r="E1380">
         <v>13145</v>
       </c>
       <c r="F1380" t="s">
@@ -63725,7 +63730,7 @@
       <c r="D1381" t="s">
         <v>1463</v>
       </c>
-      <c r="E1381" s="4">
+      <c r="E1381">
         <v>13419</v>
       </c>
       <c r="F1381" t="s">
@@ -63766,7 +63771,7 @@
       <c r="D1382" t="s">
         <v>1464</v>
       </c>
-      <c r="E1382" s="4">
+      <c r="E1382">
         <v>14131</v>
       </c>
       <c r="F1382" t="s">
@@ -63804,7 +63809,7 @@
       <c r="D1383" t="s">
         <v>1464</v>
       </c>
-      <c r="E1383" s="4">
+      <c r="E1383">
         <v>14344</v>
       </c>
       <c r="F1383" t="s">
@@ -63845,7 +63850,7 @@
       <c r="D1384" t="s">
         <v>1464</v>
       </c>
-      <c r="E1384" s="4">
+      <c r="E1384">
         <v>14388</v>
       </c>
       <c r="F1384" t="s">
@@ -63883,7 +63888,7 @@
       <c r="D1385" t="s">
         <v>1463</v>
       </c>
-      <c r="E1385" s="4">
+      <c r="E1385">
         <v>14811</v>
       </c>
       <c r="F1385" t="s">
@@ -63921,7 +63926,7 @@
       <c r="D1386" t="s">
         <v>1463</v>
       </c>
-      <c r="E1386" s="4">
+      <c r="E1386">
         <v>15279</v>
       </c>
       <c r="F1386" t="s">
@@ -63962,7 +63967,7 @@
       <c r="D1387" t="s">
         <v>1463</v>
       </c>
-      <c r="E1387" s="4">
+      <c r="E1387">
         <v>15351</v>
       </c>
       <c r="F1387" t="s">
@@ -64000,7 +64005,7 @@
       <c r="D1388" t="s">
         <v>1463</v>
       </c>
-      <c r="E1388" s="4">
+      <c r="E1388">
         <v>15564</v>
       </c>
       <c r="F1388" t="s">
@@ -64038,7 +64043,7 @@
       <c r="D1389" t="s">
         <v>1463</v>
       </c>
-      <c r="E1389" s="4">
+      <c r="E1389">
         <v>15676</v>
       </c>
       <c r="F1389" t="s">
@@ -64079,7 +64084,7 @@
       <c r="D1390" t="s">
         <v>1464</v>
       </c>
-      <c r="E1390" s="4">
+      <c r="E1390">
         <v>16442</v>
       </c>
       <c r="F1390" t="s">
@@ -64120,7 +64125,7 @@
       <c r="D1391" t="s">
         <v>1463</v>
       </c>
-      <c r="E1391" s="4">
+      <c r="E1391">
         <v>16885</v>
       </c>
       <c r="F1391" t="s">
@@ -64158,7 +64163,7 @@
       <c r="D1392" t="s">
         <v>1464</v>
       </c>
-      <c r="E1392" s="4">
+      <c r="E1392">
         <v>1737</v>
       </c>
       <c r="F1392" t="s">
@@ -64196,7 +64201,7 @@
       <c r="D1393" t="s">
         <v>1464</v>
       </c>
-      <c r="E1393" s="4">
+      <c r="E1393">
         <v>18607</v>
       </c>
       <c r="F1393" t="s">
@@ -64237,7 +64242,7 @@
       <c r="D1394" t="s">
         <v>1463</v>
       </c>
-      <c r="E1394" s="4">
+      <c r="E1394">
         <v>18722</v>
       </c>
       <c r="F1394" t="s">
@@ -64275,7 +64280,7 @@
       <c r="D1395" t="s">
         <v>1464</v>
       </c>
-      <c r="E1395" s="4">
+      <c r="E1395">
         <v>1904</v>
       </c>
       <c r="F1395" t="s">
@@ -64313,7 +64318,7 @@
       <c r="D1396" t="s">
         <v>1464</v>
       </c>
-      <c r="E1396" s="4">
+      <c r="E1396">
         <v>1908</v>
       </c>
       <c r="F1396" t="s">
@@ -64351,7 +64356,7 @@
       <c r="D1397" t="s">
         <v>1463</v>
       </c>
-      <c r="E1397" s="4">
+      <c r="E1397">
         <v>19198</v>
       </c>
       <c r="F1397" t="s">
@@ -64392,7 +64397,7 @@
       <c r="D1398" t="s">
         <v>1463</v>
       </c>
-      <c r="E1398" s="4">
+      <c r="E1398">
         <v>19251</v>
       </c>
       <c r="F1398" t="s">
@@ -64433,7 +64438,7 @@
       <c r="D1399" t="s">
         <v>1464</v>
       </c>
-      <c r="E1399" s="4">
+      <c r="E1399">
         <v>19254</v>
       </c>
       <c r="F1399" t="s">
@@ -64471,7 +64476,7 @@
       <c r="D1400" t="s">
         <v>1464</v>
       </c>
-      <c r="E1400" s="4">
+      <c r="E1400">
         <v>1930</v>
       </c>
       <c r="F1400" t="s">
@@ -64509,7 +64514,7 @@
       <c r="D1401" t="s">
         <v>1463</v>
       </c>
-      <c r="E1401" s="4">
+      <c r="E1401">
         <v>19703</v>
       </c>
       <c r="F1401" t="s">
@@ -64547,7 +64552,7 @@
       <c r="D1402" t="s">
         <v>1464</v>
       </c>
-      <c r="E1402" s="4">
+      <c r="E1402">
         <v>2154</v>
       </c>
       <c r="F1402" t="s">
@@ -64585,7 +64590,7 @@
       <c r="D1403" t="s">
         <v>1464</v>
       </c>
-      <c r="E1403" s="4">
+      <c r="E1403">
         <v>2167</v>
       </c>
       <c r="F1403" t="s">
@@ -64623,7 +64628,7 @@
       <c r="D1404" t="s">
         <v>1464</v>
       </c>
-      <c r="E1404" s="4">
+      <c r="E1404">
         <v>2231</v>
       </c>
       <c r="F1404" t="s">
@@ -64661,7 +64666,7 @@
       <c r="D1405" t="s">
         <v>1463</v>
       </c>
-      <c r="E1405" s="4">
+      <c r="E1405">
         <v>2280</v>
       </c>
       <c r="F1405" t="s">
@@ -64699,7 +64704,7 @@
       <c r="D1406" t="s">
         <v>1465</v>
       </c>
-      <c r="E1406" s="4">
+      <c r="E1406">
         <v>2396</v>
       </c>
       <c r="F1406" t="s">
@@ -64740,7 +64745,7 @@
       <c r="D1407" t="s">
         <v>1464</v>
       </c>
-      <c r="E1407" s="4">
+      <c r="E1407">
         <v>2530</v>
       </c>
       <c r="F1407" t="s">
@@ -64778,7 +64783,7 @@
       <c r="D1408" t="s">
         <v>1464</v>
       </c>
-      <c r="E1408" s="4">
+      <c r="E1408">
         <v>3086</v>
       </c>
       <c r="F1408" t="s">
@@ -64816,7 +64821,7 @@
       <c r="D1409" t="s">
         <v>1463</v>
       </c>
-      <c r="E1409" s="4">
+      <c r="E1409">
         <v>3361</v>
       </c>
       <c r="F1409" t="s">
@@ -79518,6 +79523,47 @@
       </c>
       <c r="M1779" t="s">
         <v>3310</v>
+      </c>
+    </row>
+    <row r="1780" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1780" t="s">
+        <v>3313</v>
+      </c>
+      <c r="B1780" t="s">
+        <v>1432</v>
+      </c>
+      <c r="C1780" t="s">
+        <v>1462</v>
+      </c>
+      <c r="D1780" t="s">
+        <v>1465</v>
+      </c>
+      <c r="E1780">
+        <v>21009</v>
+      </c>
+      <c r="F1780" t="s">
+        <v>3313</v>
+      </c>
+      <c r="G1780" t="s">
+        <v>3229</v>
+      </c>
+      <c r="H1780" t="s">
+        <v>3313</v>
+      </c>
+      <c r="I1780" t="s">
+        <v>3313</v>
+      </c>
+      <c r="J1780" t="s">
+        <v>3313</v>
+      </c>
+      <c r="K1780">
+        <v>660844</v>
+      </c>
+      <c r="L1780" t="s">
+        <v>3313</v>
+      </c>
+      <c r="M1780" t="s">
+        <v>3313</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating daily files July 29
</commit_message>
<xml_diff>
--- a/assets/My_Hitter_Listing.xlsx
+++ b/assets/My_Hitter_Listing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Python\dash\dashenv\github\matchup\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86D21ADD-BC67-4368-87DE-AE1AE6BAFF42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E9B7DE-EDAB-4C86-89F4-0CD13D54C0B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -10367,8 +10367,8 @@
   <dimension ref="A1:M1780"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1756" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1780" sqref="A1780"/>
+      <pane ySplit="1" topLeftCell="A227" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D240" sqref="D240"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19690,10 +19690,10 @@
         <v>662</v>
       </c>
       <c r="B240" t="s">
-        <v>3174</v>
+        <v>1413</v>
       </c>
       <c r="C240" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
       <c r="D240" t="s">
         <v>1464</v>
@@ -46260,10 +46260,10 @@
         <v>574</v>
       </c>
       <c r="B929" t="s">
-        <v>1423</v>
+        <v>1417</v>
       </c>
       <c r="C929" t="s">
-        <v>1453</v>
+        <v>1447</v>
       </c>
       <c r="D929" t="s">
         <v>1463</v>

</xml_diff>

<commit_message>
Updating files for July 30
</commit_message>
<xml_diff>
--- a/assets/My_Hitter_Listing.xlsx
+++ b/assets/My_Hitter_Listing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27920"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Python\dash\dashenv\github\matchup\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E9B7DE-EDAB-4C86-89F4-0CD13D54C0B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00E146FB-C784-46EF-9AC2-E159889EB7FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Players" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20771" uniqueCount="3314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20782" uniqueCount="3315">
   <si>
     <t>mlb_name</t>
   </si>
@@ -9975,6 +9975,9 @@
   </si>
   <si>
     <t>Leo Rivas</t>
+  </si>
+  <si>
+    <t>Dillon Dingler</t>
   </si>
 </sst>
 </file>
@@ -10364,11 +10367,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:M1780"/>
+  <dimension ref="A1:M1781"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A227" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D240" sqref="D240"/>
+      <pane ySplit="1" topLeftCell="A1156" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B1164" sqref="B1164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13232,10 +13235,10 @@
         <v>46</v>
       </c>
       <c r="B73" t="s">
-        <v>1411</v>
+        <v>1422</v>
       </c>
       <c r="C73" t="s">
-        <v>1440</v>
+        <v>1452</v>
       </c>
       <c r="D73" t="s">
         <v>1463</v>
@@ -23104,10 +23107,10 @@
         <v>846</v>
       </c>
       <c r="B328" t="s">
-        <v>3174</v>
+        <v>1405</v>
       </c>
       <c r="C328" t="s">
-        <v>1443</v>
+        <v>1434</v>
       </c>
       <c r="D328" t="s">
         <v>1463</v>
@@ -26342,10 +26345,10 @@
         <v>1263</v>
       </c>
       <c r="B411" t="s">
-        <v>1415</v>
+        <v>1427</v>
       </c>
       <c r="C411" t="s">
-        <v>1445</v>
+        <v>1457</v>
       </c>
       <c r="D411" t="s">
         <v>1463</v>
@@ -35267,10 +35270,10 @@
         <v>729</v>
       </c>
       <c r="B644" t="s">
-        <v>1420</v>
+        <v>1408</v>
       </c>
       <c r="C644" t="s">
-        <v>1450</v>
+        <v>1437</v>
       </c>
       <c r="D644" t="s">
         <v>1463</v>
@@ -48519,10 +48522,10 @@
         <v>792</v>
       </c>
       <c r="B987" t="s">
-        <v>1429</v>
+        <v>1432</v>
       </c>
       <c r="C987" t="s">
-        <v>1459</v>
+        <v>1462</v>
       </c>
       <c r="D987" t="s">
         <v>1463</v>
@@ -54540,10 +54543,10 @@
         <v>1298</v>
       </c>
       <c r="B1143" t="s">
-        <v>1432</v>
+        <v>1409</v>
       </c>
       <c r="C1143" t="s">
-        <v>1462</v>
+        <v>1438</v>
       </c>
       <c r="D1143" t="s">
         <v>1463</v>
@@ -55306,10 +55309,10 @@
         <v>1272</v>
       </c>
       <c r="B1163" t="s">
-        <v>1424</v>
+        <v>3174</v>
       </c>
       <c r="C1163" t="s">
-        <v>1454</v>
+        <v>1443</v>
       </c>
       <c r="D1163" t="s">
         <v>1464</v>
@@ -63681,10 +63684,10 @@
         <v>749</v>
       </c>
       <c r="B1380" t="s">
-        <v>1416</v>
+        <v>1421</v>
       </c>
       <c r="C1380" t="s">
-        <v>1446</v>
+        <v>1451</v>
       </c>
       <c r="D1380" t="s">
         <v>1465</v>
@@ -69555,10 +69558,10 @@
         <v>2985</v>
       </c>
       <c r="B1531" t="s">
-        <v>1410</v>
+        <v>1415</v>
       </c>
       <c r="C1531" t="s">
-        <v>1439</v>
+        <v>1445</v>
       </c>
       <c r="D1531" t="s">
         <v>1463</v>
@@ -72330,10 +72333,10 @@
         <v>3059</v>
       </c>
       <c r="B1600" t="s">
-        <v>1417</v>
+        <v>1423</v>
       </c>
       <c r="C1600" t="s">
-        <v>1447</v>
+        <v>1453</v>
       </c>
       <c r="D1600" t="s">
         <v>1463</v>
@@ -75148,10 +75151,10 @@
         <v>3183</v>
       </c>
       <c r="B1671" t="s">
-        <v>1422</v>
+        <v>1429</v>
       </c>
       <c r="C1671" t="s">
-        <v>1452</v>
+        <v>1459</v>
       </c>
       <c r="D1671" t="s">
         <v>1464</v>
@@ -79564,6 +79567,44 @@
       </c>
       <c r="M1780" t="s">
         <v>3313</v>
+      </c>
+    </row>
+    <row r="1781" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1781" t="s">
+        <v>3314</v>
+      </c>
+      <c r="B1781" t="s">
+        <v>1430</v>
+      </c>
+      <c r="C1781" t="s">
+        <v>1460</v>
+      </c>
+      <c r="D1781" t="s">
+        <v>1463</v>
+      </c>
+      <c r="E1781">
+        <v>27464</v>
+      </c>
+      <c r="F1781" t="s">
+        <v>3314</v>
+      </c>
+      <c r="G1781" t="s">
+        <v>1397</v>
+      </c>
+      <c r="H1781" t="s">
+        <v>3314</v>
+      </c>
+      <c r="I1781" t="s">
+        <v>3314</v>
+      </c>
+      <c r="J1781" t="s">
+        <v>3314</v>
+      </c>
+      <c r="L1781" t="s">
+        <v>3314</v>
+      </c>
+      <c r="M1781" t="s">
+        <v>3314</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating files for July 31
</commit_message>
<xml_diff>
--- a/assets/My_Hitter_Listing.xlsx
+++ b/assets/My_Hitter_Listing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Python\dash\dashenv\github\matchup\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00E146FB-C784-46EF-9AC2-E159889EB7FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10C107DF-A97E-49C2-AC1A-625F675C2909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Players" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20782" uniqueCount="3315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20794" uniqueCount="3317">
   <si>
     <t>mlb_name</t>
   </si>
@@ -9978,6 +9978,12 @@
   </si>
   <si>
     <t>Dillon Dingler</t>
+  </si>
+  <si>
+    <t>Pedro Leon</t>
+  </si>
+  <si>
+    <t>sa3014838</t>
   </si>
 </sst>
 </file>
@@ -10367,11 +10373,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:M1781"/>
+  <dimension ref="A1:M1782"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1156" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1164" sqref="B1164"/>
+      <pane ySplit="1" topLeftCell="A747" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B761" sqref="B761"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13156,10 +13162,10 @@
         <v>74</v>
       </c>
       <c r="B71" t="s">
-        <v>1423</v>
+        <v>1410</v>
       </c>
       <c r="C71" t="s">
-        <v>1453</v>
+        <v>1439</v>
       </c>
       <c r="D71" t="s">
         <v>1463</v>
@@ -13589,10 +13595,10 @@
         <v>1060</v>
       </c>
       <c r="B82" t="s">
-        <v>1415</v>
+        <v>1426</v>
       </c>
       <c r="C82" t="s">
-        <v>1445</v>
+        <v>1456</v>
       </c>
       <c r="D82" t="s">
         <v>1463</v>
@@ -38609,10 +38615,10 @@
         <v>239</v>
       </c>
       <c r="B730" t="s">
-        <v>1430</v>
+        <v>1407</v>
       </c>
       <c r="C730" t="s">
-        <v>1460</v>
+        <v>1436</v>
       </c>
       <c r="D730" t="s">
         <v>1463</v>
@@ -39770,10 +39776,10 @@
         <v>353</v>
       </c>
       <c r="B760" t="s">
-        <v>1429</v>
+        <v>1431</v>
       </c>
       <c r="C760" t="s">
-        <v>1459</v>
+        <v>1461</v>
       </c>
       <c r="D760" t="s">
         <v>1463</v>
@@ -52037,10 +52043,10 @@
         <v>1331</v>
       </c>
       <c r="B1078" t="s">
-        <v>1418</v>
+        <v>1408</v>
       </c>
       <c r="C1078" t="s">
-        <v>1448</v>
+        <v>1437</v>
       </c>
       <c r="D1078" t="s">
         <v>1463</v>
@@ -66951,10 +66957,10 @@
         <v>2912</v>
       </c>
       <c r="B1465" t="s">
-        <v>1416</v>
+        <v>1412</v>
       </c>
       <c r="C1465" t="s">
-        <v>1446</v>
+        <v>1441</v>
       </c>
       <c r="D1465" t="s">
         <v>1463</v>
@@ -71774,10 +71780,10 @@
         <v>3045</v>
       </c>
       <c r="B1586" t="s">
-        <v>1414</v>
+        <v>1416</v>
       </c>
       <c r="C1586" t="s">
-        <v>1444</v>
+        <v>1446</v>
       </c>
       <c r="D1586" t="s">
         <v>1464</v>
@@ -71799,6 +71805,9 @@
       </c>
       <c r="J1586" t="s">
         <v>3045</v>
+      </c>
+      <c r="K1586">
+        <v>669065</v>
       </c>
       <c r="L1586" t="s">
         <v>3045</v>
@@ -79605,6 +79614,47 @@
       </c>
       <c r="M1781" t="s">
         <v>3314</v>
+      </c>
+    </row>
+    <row r="1782" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1782" t="s">
+        <v>3315</v>
+      </c>
+      <c r="B1782" t="s">
+        <v>1422</v>
+      </c>
+      <c r="C1782" t="s">
+        <v>1452</v>
+      </c>
+      <c r="D1782" t="s">
+        <v>1463</v>
+      </c>
+      <c r="E1782" t="s">
+        <v>3316</v>
+      </c>
+      <c r="F1782" t="s">
+        <v>3315</v>
+      </c>
+      <c r="G1782" t="s">
+        <v>1398</v>
+      </c>
+      <c r="H1782" t="s">
+        <v>3315</v>
+      </c>
+      <c r="I1782" t="s">
+        <v>3315</v>
+      </c>
+      <c r="J1782" t="s">
+        <v>3315</v>
+      </c>
+      <c r="K1782">
+        <v>694175</v>
+      </c>
+      <c r="L1782" t="s">
+        <v>3315</v>
+      </c>
+      <c r="M1782" t="s">
+        <v>3315</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating files for Aug 1
</commit_message>
<xml_diff>
--- a/assets/My_Hitter_Listing.xlsx
+++ b/assets/My_Hitter_Listing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Python\dash\dashenv\github\matchup\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10C107DF-A97E-49C2-AC1A-625F675C2909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9642835-3E4B-4338-8FE8-A77B5D084778}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -10376,8 +10376,8 @@
   <dimension ref="A1:M1782"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A747" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B761" sqref="B761"/>
+      <pane ySplit="1" topLeftCell="A1665" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K1679" sqref="K1679"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -75429,10 +75429,10 @@
         <v>3190</v>
       </c>
       <c r="B1678" t="s">
-        <v>1408</v>
+        <v>1416</v>
       </c>
       <c r="C1678" t="s">
-        <v>1437</v>
+        <v>1446</v>
       </c>
       <c r="D1678" t="s">
         <v>1464</v>
@@ -75454,6 +75454,9 @@
       </c>
       <c r="J1678" t="s">
         <v>3190</v>
+      </c>
+      <c r="K1678">
+        <v>657088</v>
       </c>
       <c r="L1678" t="s">
         <v>3190</v>

</xml_diff>

<commit_message>
Updating files for Aug 4
</commit_message>
<xml_diff>
--- a/assets/My_Hitter_Listing.xlsx
+++ b/assets/My_Hitter_Listing.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27920"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Python\dash\dashenv\github\matchup\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9642835-3E4B-4338-8FE8-A77B5D084778}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CA71B30-5144-4CE3-B402-798D5FA03927}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20794" uniqueCount="3317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20848" uniqueCount="3321">
   <si>
     <t>mlb_name</t>
   </si>
@@ -9983,7 +9983,19 @@
     <t>Pedro Leon</t>
   </si>
   <si>
-    <t>sa3014838</t>
+    <t>Nick Sogard</t>
+  </si>
+  <si>
+    <t>Coby Mayo</t>
+  </si>
+  <si>
+    <t>Kameron Misner</t>
+  </si>
+  <si>
+    <t>Jerar Encarnacion</t>
+  </si>
+  <si>
+    <t>Luis De Los Santos</t>
   </si>
 </sst>
 </file>
@@ -10373,11 +10385,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:M1782"/>
+  <dimension ref="A1:M1787"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1665" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K1679" sqref="K1679"/>
+      <pane ySplit="1" topLeftCell="A1543" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B1557" sqref="B1557"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15923,10 +15935,10 @@
         <v>2806</v>
       </c>
       <c r="B142" t="s">
-        <v>1427</v>
+        <v>1423</v>
       </c>
       <c r="C142" t="s">
-        <v>1457</v>
+        <v>1453</v>
       </c>
       <c r="D142" t="s">
         <v>1465</v>
@@ -22451,10 +22463,10 @@
         <v>127</v>
       </c>
       <c r="B311" t="s">
-        <v>1409</v>
+        <v>1414</v>
       </c>
       <c r="C311" t="s">
-        <v>1438</v>
+        <v>1444</v>
       </c>
       <c r="D311" t="s">
         <v>1463</v>
@@ -23502,10 +23514,10 @@
         <v>455</v>
       </c>
       <c r="B338" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="C338" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
       <c r="D338" t="s">
         <v>1463</v>
@@ -34027,10 +34039,10 @@
         <v>331</v>
       </c>
       <c r="B612" t="s">
-        <v>1418</v>
+        <v>1416</v>
       </c>
       <c r="C612" t="s">
-        <v>1448</v>
+        <v>1446</v>
       </c>
       <c r="D612" t="s">
         <v>1463</v>
@@ -36398,10 +36410,10 @@
         <v>576</v>
       </c>
       <c r="B673" t="s">
-        <v>1429</v>
+        <v>1412</v>
       </c>
       <c r="C673" t="s">
-        <v>1459</v>
+        <v>1441</v>
       </c>
       <c r="D673" t="s">
         <v>1463</v>
@@ -70583,10 +70595,10 @@
         <v>3010</v>
       </c>
       <c r="B1556" t="s">
-        <v>1422</v>
+        <v>1416</v>
       </c>
       <c r="C1556" t="s">
-        <v>1452</v>
+        <v>1446</v>
       </c>
       <c r="D1556" t="s">
         <v>1463</v>
@@ -79612,6 +79624,9 @@
       <c r="J1781" t="s">
         <v>3314</v>
       </c>
+      <c r="K1781">
+        <v>693307</v>
+      </c>
       <c r="L1781" t="s">
         <v>3314</v>
       </c>
@@ -79632,8 +79647,8 @@
       <c r="D1782" t="s">
         <v>1463</v>
       </c>
-      <c r="E1782" t="s">
-        <v>3316</v>
+      <c r="E1782">
+        <v>27781</v>
       </c>
       <c r="F1782" t="s">
         <v>3315</v>
@@ -79658,6 +79673,211 @@
       </c>
       <c r="M1782" t="s">
         <v>3315</v>
+      </c>
+    </row>
+    <row r="1783" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1783" t="s">
+        <v>3316</v>
+      </c>
+      <c r="B1783" t="s">
+        <v>1431</v>
+      </c>
+      <c r="C1783" t="s">
+        <v>1461</v>
+      </c>
+      <c r="D1783" t="s">
+        <v>1465</v>
+      </c>
+      <c r="E1783">
+        <v>25483</v>
+      </c>
+      <c r="F1783" t="s">
+        <v>3316</v>
+      </c>
+      <c r="G1783" t="s">
+        <v>2760</v>
+      </c>
+      <c r="H1783" t="s">
+        <v>3316</v>
+      </c>
+      <c r="I1783" t="s">
+        <v>3316</v>
+      </c>
+      <c r="J1783" t="s">
+        <v>3316</v>
+      </c>
+      <c r="K1783">
+        <v>686765</v>
+      </c>
+      <c r="L1783" t="s">
+        <v>3316</v>
+      </c>
+      <c r="M1783" t="s">
+        <v>3316</v>
+      </c>
+    </row>
+    <row r="1784" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1784" t="s">
+        <v>3317</v>
+      </c>
+      <c r="B1784" t="s">
+        <v>1414</v>
+      </c>
+      <c r="C1784" t="s">
+        <v>1444</v>
+      </c>
+      <c r="D1784" t="s">
+        <v>1463</v>
+      </c>
+      <c r="E1784">
+        <v>28312</v>
+      </c>
+      <c r="F1784" t="s">
+        <v>3317</v>
+      </c>
+      <c r="G1784" t="s">
+        <v>1400</v>
+      </c>
+      <c r="H1784" t="s">
+        <v>3317</v>
+      </c>
+      <c r="I1784" t="s">
+        <v>3317</v>
+      </c>
+      <c r="J1784" t="s">
+        <v>3317</v>
+      </c>
+      <c r="K1784">
+        <v>691723</v>
+      </c>
+      <c r="L1784" t="s">
+        <v>3317</v>
+      </c>
+      <c r="M1784" t="s">
+        <v>3317</v>
+      </c>
+    </row>
+    <row r="1785" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1785" t="s">
+        <v>3318</v>
+      </c>
+      <c r="B1785" t="s">
+        <v>1423</v>
+      </c>
+      <c r="C1785" t="s">
+        <v>1453</v>
+      </c>
+      <c r="D1785" t="s">
+        <v>1464</v>
+      </c>
+      <c r="E1785">
+        <v>26374</v>
+      </c>
+      <c r="F1785" t="s">
+        <v>3318</v>
+      </c>
+      <c r="G1785" t="s">
+        <v>1398</v>
+      </c>
+      <c r="H1785" t="s">
+        <v>3318</v>
+      </c>
+      <c r="I1785" t="s">
+        <v>3318</v>
+      </c>
+      <c r="J1785" t="s">
+        <v>3318</v>
+      </c>
+      <c r="K1785">
+        <v>670244</v>
+      </c>
+      <c r="L1785" t="s">
+        <v>3318</v>
+      </c>
+      <c r="M1785" t="s">
+        <v>3318</v>
+      </c>
+    </row>
+    <row r="1786" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1786" t="s">
+        <v>3319</v>
+      </c>
+      <c r="B1786" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C1786" t="s">
+        <v>1450</v>
+      </c>
+      <c r="D1786" t="s">
+        <v>1463</v>
+      </c>
+      <c r="E1786">
+        <v>21871</v>
+      </c>
+      <c r="F1786" t="s">
+        <v>3319</v>
+      </c>
+      <c r="G1786" t="s">
+        <v>1398</v>
+      </c>
+      <c r="H1786" t="s">
+        <v>3319</v>
+      </c>
+      <c r="I1786" t="s">
+        <v>3319</v>
+      </c>
+      <c r="J1786" t="s">
+        <v>3319</v>
+      </c>
+      <c r="K1786">
+        <v>666464</v>
+      </c>
+      <c r="L1786" t="s">
+        <v>3319</v>
+      </c>
+      <c r="M1786" t="s">
+        <v>3319</v>
+      </c>
+    </row>
+    <row r="1787" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1787" t="s">
+        <v>3320</v>
+      </c>
+      <c r="B1787" t="s">
+        <v>1429</v>
+      </c>
+      <c r="C1787" t="s">
+        <v>1459</v>
+      </c>
+      <c r="D1787" t="s">
+        <v>1463</v>
+      </c>
+      <c r="E1787">
+        <v>21682</v>
+      </c>
+      <c r="F1787" t="s">
+        <v>3320</v>
+      </c>
+      <c r="G1787" t="s">
+        <v>1400</v>
+      </c>
+      <c r="H1787" t="s">
+        <v>3320</v>
+      </c>
+      <c r="I1787" t="s">
+        <v>3320</v>
+      </c>
+      <c r="J1787" t="s">
+        <v>3320</v>
+      </c>
+      <c r="K1787">
+        <v>665782</v>
+      </c>
+      <c r="L1787" t="s">
+        <v>3320</v>
+      </c>
+      <c r="M1787" t="s">
+        <v>3320</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update files for August 9
</commit_message>
<xml_diff>
--- a/assets/My_Hitter_Listing.xlsx
+++ b/assets/My_Hitter_Listing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Python\dash\dashenv\github\matchup\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{929CE05A-3D4D-4159-B5A5-BC76CE1FB053}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4197B97E-653B-4EAA-B434-E6AF11090667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20848" uniqueCount="3321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20882" uniqueCount="3325">
   <si>
     <t>mlb_name</t>
   </si>
@@ -9996,6 +9996,18 @@
   </si>
   <si>
     <t>Luis De Los Santos</t>
+  </si>
+  <si>
+    <t>Zach Dezenzo</t>
+  </si>
+  <si>
+    <t>Adrian Del Castillo</t>
+  </si>
+  <si>
+    <t>sa3016957</t>
+  </si>
+  <si>
+    <t>Charles Leblanc</t>
   </si>
 </sst>
 </file>
@@ -10385,11 +10397,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:M1787"/>
+  <dimension ref="A1:M1790"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A169" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B183" sqref="B183"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1766" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q1790" sqref="Q1790"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16980,10 +16992,10 @@
         <v>814</v>
       </c>
       <c r="B169" t="s">
-        <v>1429</v>
+        <v>1410</v>
       </c>
       <c r="C169" t="s">
-        <v>1459</v>
+        <v>1439</v>
       </c>
       <c r="D169" t="s">
         <v>1464</v>
@@ -34117,10 +34129,10 @@
         <v>395</v>
       </c>
       <c r="B614" t="s">
-        <v>1420</v>
+        <v>1416</v>
       </c>
       <c r="C614" t="s">
-        <v>1450</v>
+        <v>1446</v>
       </c>
       <c r="D614" t="s">
         <v>1463</v>
@@ -79878,6 +79890,129 @@
       </c>
       <c r="M1787" t="s">
         <v>3320</v>
+      </c>
+    </row>
+    <row r="1788" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1788" t="s">
+        <v>3321</v>
+      </c>
+      <c r="B1788" t="s">
+        <v>1422</v>
+      </c>
+      <c r="C1788" t="s">
+        <v>1452</v>
+      </c>
+      <c r="D1788" t="s">
+        <v>1463</v>
+      </c>
+      <c r="E1788">
+        <v>31562</v>
+      </c>
+      <c r="F1788" t="s">
+        <v>3321</v>
+      </c>
+      <c r="G1788" t="s">
+        <v>1402</v>
+      </c>
+      <c r="H1788" t="s">
+        <v>3321</v>
+      </c>
+      <c r="I1788" t="s">
+        <v>3321</v>
+      </c>
+      <c r="J1788" t="s">
+        <v>3321</v>
+      </c>
+      <c r="K1788">
+        <v>701305</v>
+      </c>
+      <c r="L1788" t="s">
+        <v>3321</v>
+      </c>
+      <c r="M1788" t="s">
+        <v>3321</v>
+      </c>
+    </row>
+    <row r="1789" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1789" t="s">
+        <v>3322</v>
+      </c>
+      <c r="B1789" t="s">
+        <v>1421</v>
+      </c>
+      <c r="C1789" t="s">
+        <v>1451</v>
+      </c>
+      <c r="D1789" t="s">
+        <v>1464</v>
+      </c>
+      <c r="E1789" t="s">
+        <v>3323</v>
+      </c>
+      <c r="F1789" t="s">
+        <v>3322</v>
+      </c>
+      <c r="G1789" t="s">
+        <v>1397</v>
+      </c>
+      <c r="H1789" t="s">
+        <v>3322</v>
+      </c>
+      <c r="I1789" t="s">
+        <v>3322</v>
+      </c>
+      <c r="J1789" t="s">
+        <v>3322</v>
+      </c>
+      <c r="K1789">
+        <v>680728</v>
+      </c>
+      <c r="L1789" t="s">
+        <v>3322</v>
+      </c>
+      <c r="M1789" t="s">
+        <v>3322</v>
+      </c>
+    </row>
+    <row r="1790" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1790" t="s">
+        <v>3324</v>
+      </c>
+      <c r="B1790" t="s">
+        <v>1404</v>
+      </c>
+      <c r="C1790" t="s">
+        <v>1433</v>
+      </c>
+      <c r="D1790" t="s">
+        <v>1463</v>
+      </c>
+      <c r="E1790">
+        <v>19813</v>
+      </c>
+      <c r="F1790" t="s">
+        <v>3324</v>
+      </c>
+      <c r="G1790" t="s">
+        <v>2764</v>
+      </c>
+      <c r="H1790" t="s">
+        <v>3324</v>
+      </c>
+      <c r="I1790" t="s">
+        <v>3324</v>
+      </c>
+      <c r="J1790" t="s">
+        <v>3324</v>
+      </c>
+      <c r="K1790">
+        <v>641779</v>
+      </c>
+      <c r="L1790" t="s">
+        <v>3324</v>
+      </c>
+      <c r="M1790" t="s">
+        <v>3324</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating daily files for August 16
</commit_message>
<xml_diff>
--- a/assets/My_Hitter_Listing.xlsx
+++ b/assets/My_Hitter_Listing.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28011"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Python\dash\dashenv\github\matchup\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4197B97E-653B-4EAA-B434-E6AF11090667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F5C31B1-368F-4DAA-BDEA-A56CFFD729E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20882" uniqueCount="3325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20928" uniqueCount="3331">
   <si>
     <t>mlb_name</t>
   </si>
@@ -10008,6 +10008,24 @@
   </si>
   <si>
     <t>Charles Leblanc</t>
+  </si>
+  <si>
+    <t>Andres Chaparro</t>
+  </si>
+  <si>
+    <t>Junior Caminero</t>
+  </si>
+  <si>
+    <t>Trey Sweeney</t>
+  </si>
+  <si>
+    <t>sa3016973</t>
+  </si>
+  <si>
+    <t>Jace Jung</t>
+  </si>
+  <si>
+    <t>sa3019992</t>
   </si>
 </sst>
 </file>
@@ -10397,11 +10415,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:M1790"/>
+  <dimension ref="A1:M1794"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1766" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q1790" sqref="Q1790"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1770" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G1794" sqref="G1794"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -75532,10 +75550,10 @@
         <v>3192</v>
       </c>
       <c r="B1680" t="s">
-        <v>1422</v>
+        <v>1429</v>
       </c>
       <c r="C1680" t="s">
-        <v>1452</v>
+        <v>1459</v>
       </c>
       <c r="D1680" t="s">
         <v>1464</v>
@@ -75722,10 +75740,10 @@
         <v>3196</v>
       </c>
       <c r="B1685" t="s">
-        <v>1405</v>
+        <v>3174</v>
       </c>
       <c r="C1685" t="s">
-        <v>1434</v>
+        <v>1443</v>
       </c>
       <c r="D1685" t="s">
         <v>1464</v>
@@ -80013,6 +80031,170 @@
       </c>
       <c r="M1790" t="s">
         <v>3324</v>
+      </c>
+    </row>
+    <row r="1791" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1791" t="s">
+        <v>3326</v>
+      </c>
+      <c r="B1791" t="s">
+        <v>1423</v>
+      </c>
+      <c r="C1791" t="s">
+        <v>1453</v>
+      </c>
+      <c r="D1791" t="s">
+        <v>1463</v>
+      </c>
+      <c r="E1791">
+        <v>28163</v>
+      </c>
+      <c r="F1791" t="s">
+        <v>3326</v>
+      </c>
+      <c r="G1791" t="s">
+        <v>1400</v>
+      </c>
+      <c r="H1791" t="s">
+        <v>3326</v>
+      </c>
+      <c r="I1791" t="s">
+        <v>3326</v>
+      </c>
+      <c r="J1791" t="s">
+        <v>3326</v>
+      </c>
+      <c r="K1791">
+        <v>691406</v>
+      </c>
+      <c r="L1791" t="s">
+        <v>3326</v>
+      </c>
+      <c r="M1791" t="s">
+        <v>3326</v>
+      </c>
+    </row>
+    <row r="1792" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1792" t="s">
+        <v>3325</v>
+      </c>
+      <c r="B1792" t="s">
+        <v>3174</v>
+      </c>
+      <c r="C1792" t="s">
+        <v>1443</v>
+      </c>
+      <c r="D1792" t="s">
+        <v>1463</v>
+      </c>
+      <c r="E1792">
+        <v>21797</v>
+      </c>
+      <c r="F1792" t="s">
+        <v>3325</v>
+      </c>
+      <c r="G1792" t="s">
+        <v>1403</v>
+      </c>
+      <c r="H1792" t="s">
+        <v>3325</v>
+      </c>
+      <c r="I1792" t="s">
+        <v>3325</v>
+      </c>
+      <c r="J1792" t="s">
+        <v>3325</v>
+      </c>
+      <c r="K1792">
+        <v>665953</v>
+      </c>
+      <c r="L1792" t="s">
+        <v>3325</v>
+      </c>
+      <c r="M1792" t="s">
+        <v>3325</v>
+      </c>
+    </row>
+    <row r="1793" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1793" t="s">
+        <v>3327</v>
+      </c>
+      <c r="B1793" t="s">
+        <v>1430</v>
+      </c>
+      <c r="C1793" t="s">
+        <v>1460</v>
+      </c>
+      <c r="D1793" t="s">
+        <v>1464</v>
+      </c>
+      <c r="E1793" t="s">
+        <v>3328</v>
+      </c>
+      <c r="F1793" t="s">
+        <v>3327</v>
+      </c>
+      <c r="G1793" t="s">
+        <v>1399</v>
+      </c>
+      <c r="H1793" t="s">
+        <v>3327</v>
+      </c>
+      <c r="I1793" t="s">
+        <v>3327</v>
+      </c>
+      <c r="J1793" t="s">
+        <v>3327</v>
+      </c>
+      <c r="K1793">
+        <v>700242</v>
+      </c>
+      <c r="L1793" t="s">
+        <v>3327</v>
+      </c>
+      <c r="M1793" t="s">
+        <v>3327</v>
+      </c>
+    </row>
+    <row r="1794" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1794" t="s">
+        <v>3329</v>
+      </c>
+      <c r="B1794" t="s">
+        <v>1430</v>
+      </c>
+      <c r="C1794" t="s">
+        <v>1460</v>
+      </c>
+      <c r="D1794" t="s">
+        <v>1464</v>
+      </c>
+      <c r="E1794" t="s">
+        <v>3330</v>
+      </c>
+      <c r="F1794" t="s">
+        <v>3329</v>
+      </c>
+      <c r="G1794" t="s">
+        <v>2764</v>
+      </c>
+      <c r="H1794" t="s">
+        <v>3329</v>
+      </c>
+      <c r="I1794" t="s">
+        <v>3329</v>
+      </c>
+      <c r="J1794" t="s">
+        <v>3329</v>
+      </c>
+      <c r="K1794">
+        <v>690291</v>
+      </c>
+      <c r="L1794" t="s">
+        <v>3329</v>
+      </c>
+      <c r="M1794" t="s">
+        <v>3329</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating daily files for August 28
</commit_message>
<xml_diff>
--- a/assets/My_Hitter_Listing.xlsx
+++ b/assets/My_Hitter_Listing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Python\dash\dashenv\github\matchup\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC171AA-0213-4338-BE0F-10D45530BBB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{764ACA68-788E-47AB-B7C5-F5A7E9DA4499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1080" yWindow="1080" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Players" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20947" uniqueCount="3330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20980" uniqueCount="3333">
   <si>
     <t>mlb_name</t>
   </si>
@@ -10023,6 +10023,15 @@
   </si>
   <si>
     <t>Grant McCray</t>
+  </si>
+  <si>
+    <t>Dylan Crews</t>
+  </si>
+  <si>
+    <t>Mason McCoy</t>
+  </si>
+  <si>
+    <t>Drew Romo</t>
   </si>
 </sst>
 </file>
@@ -10098,7 +10107,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -10107,6 +10116,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -10412,11 +10422,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:M1796"/>
+  <dimension ref="A1:M1799"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A923" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O932" sqref="O932"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1791" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E1797" sqref="E1797"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13201,10 +13211,10 @@
         <v>74</v>
       </c>
       <c r="B71" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="C71" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
       <c r="D71" t="s">
         <v>1463</v>
@@ -18361,10 +18371,10 @@
         <v>133</v>
       </c>
       <c r="B204" t="s">
-        <v>1413</v>
+        <v>1422</v>
       </c>
       <c r="C204" t="s">
-        <v>1442</v>
+        <v>1452</v>
       </c>
       <c r="D204" t="s">
         <v>1464</v>
@@ -47874,10 +47884,10 @@
         <v>1258</v>
       </c>
       <c r="B969" t="s">
-        <v>1427</v>
+        <v>1410</v>
       </c>
       <c r="C969" t="s">
-        <v>1457</v>
+        <v>1439</v>
       </c>
       <c r="D969" t="s">
         <v>1465</v>
@@ -54509,10 +54519,10 @@
         <v>869</v>
       </c>
       <c r="B1141" t="s">
-        <v>1404</v>
+        <v>1421</v>
       </c>
       <c r="C1141" t="s">
-        <v>1433</v>
+        <v>1451</v>
       </c>
       <c r="D1141" t="s">
         <v>1464</v>
@@ -59695,10 +59705,10 @@
         <v>415</v>
       </c>
       <c r="B1275" t="s">
-        <v>1431</v>
+        <v>1409</v>
       </c>
       <c r="C1275" t="s">
-        <v>1461</v>
+        <v>1438</v>
       </c>
       <c r="D1275" t="s">
         <v>1464</v>
@@ -80228,6 +80238,9 @@
       <c r="J1795" t="s">
         <v>3328</v>
       </c>
+      <c r="K1795">
+        <v>694359</v>
+      </c>
       <c r="L1795" t="s">
         <v>3328</v>
       </c>
@@ -80266,11 +80279,137 @@
       <c r="J1796" t="s">
         <v>3329</v>
       </c>
+      <c r="K1796">
+        <v>687529</v>
+      </c>
       <c r="L1796" t="s">
         <v>3329</v>
       </c>
       <c r="M1796" t="s">
         <v>3329</v>
+      </c>
+    </row>
+    <row r="1797" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1797" s="4" t="s">
+        <v>3330</v>
+      </c>
+      <c r="B1797" s="4" t="s">
+        <v>3174</v>
+      </c>
+      <c r="C1797" s="4" t="s">
+        <v>1443</v>
+      </c>
+      <c r="D1797" s="4" t="s">
+        <v>1463</v>
+      </c>
+      <c r="E1797" s="4">
+        <v>33541</v>
+      </c>
+      <c r="F1797" s="4" t="s">
+        <v>3330</v>
+      </c>
+      <c r="G1797" s="4" t="s">
+        <v>1398</v>
+      </c>
+      <c r="H1797" s="4" t="s">
+        <v>3330</v>
+      </c>
+      <c r="I1797" s="4" t="s">
+        <v>3330</v>
+      </c>
+      <c r="J1797" s="4" t="s">
+        <v>3330</v>
+      </c>
+      <c r="K1797" s="4">
+        <v>686611</v>
+      </c>
+      <c r="L1797" s="4" t="s">
+        <v>3330</v>
+      </c>
+      <c r="M1797" s="4" t="s">
+        <v>3330</v>
+      </c>
+    </row>
+    <row r="1798" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1798" s="4" t="s">
+        <v>3331</v>
+      </c>
+      <c r="B1798" s="4" t="s">
+        <v>1406</v>
+      </c>
+      <c r="C1798" s="4" t="s">
+        <v>1435</v>
+      </c>
+      <c r="D1798" s="4" t="s">
+        <v>1463</v>
+      </c>
+      <c r="E1798" s="4">
+        <v>22232</v>
+      </c>
+      <c r="F1798" s="4" t="s">
+        <v>3331</v>
+      </c>
+      <c r="G1798" s="4" t="s">
+        <v>1399</v>
+      </c>
+      <c r="H1798" s="4" t="s">
+        <v>3331</v>
+      </c>
+      <c r="I1798" s="4" t="s">
+        <v>3331</v>
+      </c>
+      <c r="J1798" s="4" t="s">
+        <v>3331</v>
+      </c>
+      <c r="K1798" s="4">
+        <v>669200</v>
+      </c>
+      <c r="L1798" s="4" t="s">
+        <v>3331</v>
+      </c>
+      <c r="M1798" s="4" t="s">
+        <v>3331</v>
+      </c>
+    </row>
+    <row r="1799" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1799" s="4" t="s">
+        <v>3332</v>
+      </c>
+      <c r="B1799" s="4" t="s">
+        <v>1428</v>
+      </c>
+      <c r="C1799" s="4" t="s">
+        <v>1458</v>
+      </c>
+      <c r="D1799" s="4" t="s">
+        <v>1465</v>
+      </c>
+      <c r="E1799" s="4">
+        <v>27763</v>
+      </c>
+      <c r="F1799" s="4" t="s">
+        <v>3332</v>
+      </c>
+      <c r="G1799" s="4" t="s">
+        <v>1397</v>
+      </c>
+      <c r="H1799" s="4" t="s">
+        <v>3332</v>
+      </c>
+      <c r="I1799" s="4" t="s">
+        <v>3332</v>
+      </c>
+      <c r="J1799" s="4" t="s">
+        <v>3332</v>
+      </c>
+      <c r="K1799" s="4">
+        <v>691011</v>
+      </c>
+      <c r="L1799" s="4" t="s">
+        <v>3332</v>
+      </c>
+      <c r="M1799" s="4" t="s">
+        <v>3332</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating daily files for August 30
</commit_message>
<xml_diff>
--- a/assets/My_Hitter_Listing.xlsx
+++ b/assets/My_Hitter_Listing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Python\dash\dashenv\github\matchup\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{764ACA68-788E-47AB-B7C5-F5A7E9DA4499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20F0FF4E-6C83-4A66-B438-3A133BA5DC46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="1080" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Players" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20980" uniqueCount="3333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20991" uniqueCount="3334">
   <si>
     <t>mlb_name</t>
   </si>
@@ -10032,6 +10032,9 @@
   </si>
   <si>
     <t>Drew Romo</t>
+  </si>
+  <si>
+    <t>Tyler Gentry</t>
   </si>
 </sst>
 </file>
@@ -10107,7 +10110,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -10116,7 +10119,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -10422,11 +10424,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:M1799"/>
+  <dimension ref="A1:M1800"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1791" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1797" sqref="E1797"/>
+      <pane ySplit="1" topLeftCell="A1776" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K1801" sqref="K1801"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -28379,10 +28381,10 @@
         <v>629</v>
       </c>
       <c r="B463" t="s">
-        <v>1410</v>
+        <v>1422</v>
       </c>
       <c r="C463" t="s">
-        <v>1439</v>
+        <v>1452</v>
       </c>
       <c r="D463" t="s">
         <v>1464</v>
@@ -49583,7 +49585,7 @@
         <v>2893</v>
       </c>
       <c r="B1013" t="s">
-        <v>1416</v>
+        <v>1414</v>
       </c>
       <c r="C1013" t="s">
         <v>1446</v>
@@ -80289,127 +80291,168 @@
         <v>3329</v>
       </c>
     </row>
-    <row r="1797" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1797" s="4" t="s">
+    <row r="1797" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1797" t="s">
         <v>3330</v>
       </c>
-      <c r="B1797" s="4" t="s">
+      <c r="B1797" t="s">
         <v>3174</v>
       </c>
-      <c r="C1797" s="4" t="s">
+      <c r="C1797" t="s">
         <v>1443</v>
       </c>
-      <c r="D1797" s="4" t="s">
-        <v>1463</v>
-      </c>
-      <c r="E1797" s="4">
+      <c r="D1797" t="s">
+        <v>1463</v>
+      </c>
+      <c r="E1797">
         <v>33541</v>
       </c>
-      <c r="F1797" s="4" t="s">
+      <c r="F1797" t="s">
         <v>3330</v>
       </c>
-      <c r="G1797" s="4" t="s">
+      <c r="G1797" t="s">
         <v>1398</v>
       </c>
-      <c r="H1797" s="4" t="s">
+      <c r="H1797" t="s">
         <v>3330</v>
       </c>
-      <c r="I1797" s="4" t="s">
+      <c r="I1797" t="s">
         <v>3330</v>
       </c>
-      <c r="J1797" s="4" t="s">
+      <c r="J1797" t="s">
         <v>3330</v>
       </c>
-      <c r="K1797" s="4">
+      <c r="K1797">
         <v>686611</v>
       </c>
-      <c r="L1797" s="4" t="s">
+      <c r="L1797" t="s">
         <v>3330</v>
       </c>
-      <c r="M1797" s="4" t="s">
+      <c r="M1797" t="s">
         <v>3330</v>
       </c>
     </row>
-    <row r="1798" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1798" s="4" t="s">
+    <row r="1798" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1798" t="s">
         <v>3331</v>
       </c>
-      <c r="B1798" s="4" t="s">
+      <c r="B1798" t="s">
         <v>1406</v>
       </c>
-      <c r="C1798" s="4" t="s">
+      <c r="C1798" t="s">
         <v>1435</v>
       </c>
-      <c r="D1798" s="4" t="s">
-        <v>1463</v>
-      </c>
-      <c r="E1798" s="4">
+      <c r="D1798" t="s">
+        <v>1463</v>
+      </c>
+      <c r="E1798">
         <v>22232</v>
       </c>
-      <c r="F1798" s="4" t="s">
+      <c r="F1798" t="s">
         <v>3331</v>
       </c>
-      <c r="G1798" s="4" t="s">
+      <c r="G1798" t="s">
         <v>1399</v>
       </c>
-      <c r="H1798" s="4" t="s">
+      <c r="H1798" t="s">
         <v>3331</v>
       </c>
-      <c r="I1798" s="4" t="s">
+      <c r="I1798" t="s">
         <v>3331</v>
       </c>
-      <c r="J1798" s="4" t="s">
+      <c r="J1798" t="s">
         <v>3331</v>
       </c>
-      <c r="K1798" s="4">
+      <c r="K1798">
         <v>669200</v>
       </c>
-      <c r="L1798" s="4" t="s">
+      <c r="L1798" t="s">
         <v>3331</v>
       </c>
-      <c r="M1798" s="4" t="s">
+      <c r="M1798" t="s">
         <v>3331</v>
       </c>
     </row>
-    <row r="1799" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1799" s="4" t="s">
+    <row r="1799" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1799" t="s">
         <v>3332</v>
       </c>
-      <c r="B1799" s="4" t="s">
+      <c r="B1799" t="s">
         <v>1428</v>
       </c>
-      <c r="C1799" s="4" t="s">
+      <c r="C1799" t="s">
         <v>1458</v>
       </c>
-      <c r="D1799" s="4" t="s">
+      <c r="D1799" t="s">
         <v>1465</v>
       </c>
-      <c r="E1799" s="4">
+      <c r="E1799">
         <v>27763</v>
       </c>
-      <c r="F1799" s="4" t="s">
+      <c r="F1799" t="s">
         <v>3332</v>
       </c>
-      <c r="G1799" s="4" t="s">
+      <c r="G1799" t="s">
         <v>1397</v>
       </c>
-      <c r="H1799" s="4" t="s">
+      <c r="H1799" t="s">
         <v>3332</v>
       </c>
-      <c r="I1799" s="4" t="s">
+      <c r="I1799" t="s">
         <v>3332</v>
       </c>
-      <c r="J1799" s="4" t="s">
+      <c r="J1799" t="s">
         <v>3332</v>
       </c>
-      <c r="K1799" s="4">
+      <c r="K1799">
         <v>691011</v>
       </c>
-      <c r="L1799" s="4" t="s">
+      <c r="L1799" t="s">
         <v>3332</v>
       </c>
-      <c r="M1799" s="4" t="s">
+      <c r="M1799" t="s">
         <v>3332</v>
+      </c>
+    </row>
+    <row r="1800" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1800" t="s">
+        <v>3333</v>
+      </c>
+      <c r="B1800" t="s">
+        <v>1426</v>
+      </c>
+      <c r="C1800" t="s">
+        <v>1456</v>
+      </c>
+      <c r="D1800" t="s">
+        <v>1463</v>
+      </c>
+      <c r="E1800">
+        <v>27784</v>
+      </c>
+      <c r="F1800" t="s">
+        <v>3333</v>
+      </c>
+      <c r="G1800" t="s">
+        <v>1398</v>
+      </c>
+      <c r="H1800" t="s">
+        <v>3333</v>
+      </c>
+      <c r="I1800" t="s">
+        <v>3333</v>
+      </c>
+      <c r="J1800" t="s">
+        <v>3333</v>
+      </c>
+      <c r="K1800">
+        <v>694355</v>
+      </c>
+      <c r="L1800" t="s">
+        <v>3333</v>
+      </c>
+      <c r="M1800" t="s">
+        <v>3333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating daily files for September 2
</commit_message>
<xml_diff>
--- a/assets/My_Hitter_Listing.xlsx
+++ b/assets/My_Hitter_Listing.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28015"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Python\dash\dashenv\github\matchup\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20F0FF4E-6C83-4A66-B438-3A133BA5DC46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56189E52-6A85-43F0-A117-7F3394AEC0F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20991" uniqueCount="3334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21013" uniqueCount="3336">
   <si>
     <t>mlb_name</t>
   </si>
@@ -10035,6 +10035,12 @@
   </si>
   <si>
     <t>Tyler Gentry</t>
+  </si>
+  <si>
+    <t>Brewer Hicklen</t>
+  </si>
+  <si>
+    <t>Griffin Conine</t>
   </si>
 </sst>
 </file>
@@ -10424,11 +10430,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:M1800"/>
+  <dimension ref="A1:M1802"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1776" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K1801" sqref="K1801"/>
+      <pane ySplit="1" topLeftCell="A1000" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C1014" sqref="C1014"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -26402,10 +26408,10 @@
         <v>1263</v>
       </c>
       <c r="B411" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="C411" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
       <c r="D411" t="s">
         <v>1463</v>
@@ -49588,7 +49594,7 @@
         <v>1414</v>
       </c>
       <c r="C1013" t="s">
-        <v>1446</v>
+        <v>1444</v>
       </c>
       <c r="D1013" t="s">
         <v>1463</v>
@@ -64411,10 +64417,10 @@
         <v>1384</v>
       </c>
       <c r="B1397" t="s">
-        <v>1416</v>
+        <v>1426</v>
       </c>
       <c r="C1397" t="s">
-        <v>1446</v>
+        <v>1456</v>
       </c>
       <c r="D1397" t="s">
         <v>1463</v>
@@ -73725,10 +73731,10 @@
         <v>3138</v>
       </c>
       <c r="B1633" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
       <c r="C1633" t="s">
-        <v>1446</v>
+        <v>1445</v>
       </c>
       <c r="D1633" t="s">
         <v>1463</v>
@@ -80453,6 +80459,88 @@
       </c>
       <c r="M1800" t="s">
         <v>3333</v>
+      </c>
+    </row>
+    <row r="1801" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1801" t="s">
+        <v>3334</v>
+      </c>
+      <c r="B1801" t="s">
+        <v>1425</v>
+      </c>
+      <c r="C1801" t="s">
+        <v>1455</v>
+      </c>
+      <c r="D1801" t="s">
+        <v>1463</v>
+      </c>
+      <c r="E1801">
+        <v>20450</v>
+      </c>
+      <c r="F1801" t="s">
+        <v>3334</v>
+      </c>
+      <c r="G1801" t="s">
+        <v>1398</v>
+      </c>
+      <c r="H1801" t="s">
+        <v>3334</v>
+      </c>
+      <c r="I1801" t="s">
+        <v>3334</v>
+      </c>
+      <c r="J1801" t="s">
+        <v>3334</v>
+      </c>
+      <c r="K1801">
+        <v>676551</v>
+      </c>
+      <c r="L1801" t="s">
+        <v>3334</v>
+      </c>
+      <c r="M1801" t="s">
+        <v>3334</v>
+      </c>
+    </row>
+    <row r="1802" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1802" t="s">
+        <v>3335</v>
+      </c>
+      <c r="B1802" t="s">
+        <v>1416</v>
+      </c>
+      <c r="C1802" t="s">
+        <v>1446</v>
+      </c>
+      <c r="D1802" t="s">
+        <v>1464</v>
+      </c>
+      <c r="E1802">
+        <v>21626</v>
+      </c>
+      <c r="F1802" t="s">
+        <v>3335</v>
+      </c>
+      <c r="G1802" t="s">
+        <v>1398</v>
+      </c>
+      <c r="H1802" t="s">
+        <v>3335</v>
+      </c>
+      <c r="I1802" t="s">
+        <v>3335</v>
+      </c>
+      <c r="J1802" t="s">
+        <v>3335</v>
+      </c>
+      <c r="K1802">
+        <v>665052</v>
+      </c>
+      <c r="L1802" t="s">
+        <v>3335</v>
+      </c>
+      <c r="M1802" t="s">
+        <v>3335</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating daily files for September 4
</commit_message>
<xml_diff>
--- a/assets/My_Hitter_Listing.xlsx
+++ b/assets/My_Hitter_Listing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Python\dash\dashenv\github\matchup\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56189E52-6A85-43F0-A117-7F3394AEC0F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57ED4C31-1510-4731-9F60-436C6FFA09D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21013" uniqueCount="3336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21048" uniqueCount="3340">
   <si>
     <t>mlb_name</t>
   </si>
@@ -10041,6 +10041,18 @@
   </si>
   <si>
     <t>Griffin Conine</t>
+  </si>
+  <si>
+    <t>Michael Helman</t>
+  </si>
+  <si>
+    <t>sa123</t>
+  </si>
+  <si>
+    <t>Logan Driscoll</t>
+  </si>
+  <si>
+    <t>Tristan Gray</t>
   </si>
 </sst>
 </file>
@@ -10430,11 +10442,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:M1802"/>
+  <dimension ref="A1:M1805"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1000" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1014" sqref="C1014"/>
+      <pane ySplit="1" topLeftCell="A1781" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K1806" sqref="K1806"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -80543,6 +80555,123 @@
         <v>3335</v>
       </c>
     </row>
+    <row r="1803" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1803" t="s">
+        <v>3336</v>
+      </c>
+      <c r="B1803" t="s">
+        <v>1424</v>
+      </c>
+      <c r="C1803" t="s">
+        <v>1454</v>
+      </c>
+      <c r="D1803" t="s">
+        <v>1463</v>
+      </c>
+      <c r="E1803" t="s">
+        <v>3337</v>
+      </c>
+      <c r="F1803" t="s">
+        <v>3336</v>
+      </c>
+      <c r="G1803" t="s">
+        <v>2761</v>
+      </c>
+      <c r="H1803" t="s">
+        <v>3336</v>
+      </c>
+      <c r="I1803" t="s">
+        <v>3336</v>
+      </c>
+      <c r="J1803" t="s">
+        <v>3336</v>
+      </c>
+      <c r="L1803" t="s">
+        <v>3336</v>
+      </c>
+      <c r="M1803" t="s">
+        <v>3336</v>
+      </c>
+    </row>
+    <row r="1804" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1804" t="s">
+        <v>3338</v>
+      </c>
+      <c r="B1804" t="s">
+        <v>1423</v>
+      </c>
+      <c r="C1804" t="s">
+        <v>1453</v>
+      </c>
+      <c r="D1804" t="s">
+        <v>1464</v>
+      </c>
+      <c r="E1804" t="s">
+        <v>3337</v>
+      </c>
+      <c r="F1804" t="s">
+        <v>3338</v>
+      </c>
+      <c r="G1804" t="s">
+        <v>1397</v>
+      </c>
+      <c r="H1804" t="s">
+        <v>3338</v>
+      </c>
+      <c r="I1804" t="s">
+        <v>3338</v>
+      </c>
+      <c r="J1804" t="s">
+        <v>3338</v>
+      </c>
+      <c r="L1804" t="s">
+        <v>3338</v>
+      </c>
+      <c r="M1804" t="s">
+        <v>3338</v>
+      </c>
+    </row>
+    <row r="1805" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1805" t="s">
+        <v>3339</v>
+      </c>
+      <c r="B1805" t="s">
+        <v>1411</v>
+      </c>
+      <c r="C1805" t="s">
+        <v>1440</v>
+      </c>
+      <c r="D1805" t="s">
+        <v>1464</v>
+      </c>
+      <c r="E1805">
+        <v>19877</v>
+      </c>
+      <c r="F1805" t="s">
+        <v>3339</v>
+      </c>
+      <c r="G1805" t="s">
+        <v>1400</v>
+      </c>
+      <c r="H1805" t="s">
+        <v>3339</v>
+      </c>
+      <c r="I1805" t="s">
+        <v>3339</v>
+      </c>
+      <c r="J1805" t="s">
+        <v>3339</v>
+      </c>
+      <c r="K1805">
+        <v>656484</v>
+      </c>
+      <c r="L1805" t="s">
+        <v>3339</v>
+      </c>
+      <c r="M1805" t="s">
+        <v>3339</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I1395">
     <sortCondition ref="A2:A1395"/>

</xml_diff>

<commit_message>
Updating daily files for September 6
</commit_message>
<xml_diff>
--- a/assets/My_Hitter_Listing.xlsx
+++ b/assets/My_Hitter_Listing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Python\dash\dashenv\github\matchup\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57ED4C31-1510-4731-9F60-436C6FFA09D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D416F17C-3BA7-4E16-BE41-178A32BA8CEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1776" yWindow="1776" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Players" sheetId="1" r:id="rId1"/>
@@ -10445,8 +10445,8 @@
   <dimension ref="A1:M1805"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1781" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K1806" sqref="K1806"/>
+      <pane ySplit="1" topLeftCell="A470" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B478" sqref="B478"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -28937,10 +28937,10 @@
         <v>1115</v>
       </c>
       <c r="B477" t="s">
-        <v>1407</v>
+        <v>1426</v>
       </c>
       <c r="C477" t="s">
-        <v>1436</v>
+        <v>1456</v>
       </c>
       <c r="D477" t="s">
         <v>1465</v>

</xml_diff>

<commit_message>
Updating daily files for Sept 10
</commit_message>
<xml_diff>
--- a/assets/My_Hitter_Listing.xlsx
+++ b/assets/My_Hitter_Listing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Python\dash\dashenv\github\matchup\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2633ECD8-1708-4BFA-9038-54FF45DE7F8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBB2032A-B080-4596-96D1-3C5708BA3E37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21112" uniqueCount="3345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21135" uniqueCount="3349">
   <si>
     <t>mlb_name</t>
   </si>
@@ -10068,6 +10068,18 @@
   </si>
   <si>
     <t>Jasson Dominguez</t>
+  </si>
+  <si>
+    <t>DaShawn Keirsey</t>
+  </si>
+  <si>
+    <t>DaShawn Keirsey Jr</t>
+  </si>
+  <si>
+    <t>Thomas Saggese</t>
+  </si>
+  <si>
+    <t>sa123</t>
   </si>
 </sst>
 </file>
@@ -10464,11 +10476,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:M1811"/>
+  <dimension ref="A1:M1813"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1787" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1804" sqref="E1804"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1789" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K1804" sqref="K1804"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -68104,10 +68116,10 @@
         <v>2941</v>
       </c>
       <c r="B1492" t="s">
-        <v>1410</v>
+        <v>1413</v>
       </c>
       <c r="C1492" t="s">
-        <v>1439</v>
+        <v>1442</v>
       </c>
       <c r="D1492" t="s">
         <v>1465</v>
@@ -68129,6 +68141,9 @@
       </c>
       <c r="J1492" t="s">
         <v>2941</v>
+      </c>
+      <c r="K1492">
+        <v>657193</v>
       </c>
       <c r="L1492" t="s">
         <v>2941</v>
@@ -80608,6 +80623,9 @@
       <c r="J1803" t="s">
         <v>3336</v>
       </c>
+      <c r="K1803">
+        <v>680737</v>
+      </c>
       <c r="L1803" t="s">
         <v>3336</v>
       </c>
@@ -80646,6 +80664,9 @@
       <c r="J1804" t="s">
         <v>3337</v>
       </c>
+      <c r="K1804">
+        <v>686482</v>
+      </c>
       <c r="L1804" t="s">
         <v>3337</v>
       </c>
@@ -80930,11 +80951,96 @@
       <c r="J1811" t="s">
         <v>3344</v>
       </c>
+      <c r="K1811">
+        <v>691176</v>
+      </c>
       <c r="L1811" t="s">
         <v>3344</v>
       </c>
       <c r="M1811" t="s">
         <v>3344</v>
+      </c>
+    </row>
+    <row r="1812" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1812" t="s">
+        <v>3345</v>
+      </c>
+      <c r="B1812" t="s">
+        <v>1424</v>
+      </c>
+      <c r="C1812" t="s">
+        <v>1454</v>
+      </c>
+      <c r="D1812" t="s">
+        <v>1464</v>
+      </c>
+      <c r="E1812">
+        <v>24496</v>
+      </c>
+      <c r="F1812" t="s">
+        <v>3345</v>
+      </c>
+      <c r="G1812" t="s">
+        <v>1398</v>
+      </c>
+      <c r="H1812" t="s">
+        <v>3345</v>
+      </c>
+      <c r="I1812" t="s">
+        <v>3345</v>
+      </c>
+      <c r="J1812" t="s">
+        <v>3346</v>
+      </c>
+      <c r="K1812">
+        <v>680577</v>
+      </c>
+      <c r="L1812" t="s">
+        <v>3345</v>
+      </c>
+      <c r="M1812" t="s">
+        <v>3345</v>
+      </c>
+    </row>
+    <row r="1813" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1813" t="s">
+        <v>3347</v>
+      </c>
+      <c r="B1813" t="s">
+        <v>1427</v>
+      </c>
+      <c r="C1813" t="s">
+        <v>1457</v>
+      </c>
+      <c r="D1813" t="s">
+        <v>1463</v>
+      </c>
+      <c r="E1813" t="s">
+        <v>3348</v>
+      </c>
+      <c r="F1813" t="s">
+        <v>3347</v>
+      </c>
+      <c r="G1813" s="1" t="s">
+        <v>2763</v>
+      </c>
+      <c r="H1813" t="s">
+        <v>3347</v>
+      </c>
+      <c r="I1813" t="s">
+        <v>3347</v>
+      </c>
+      <c r="J1813" t="s">
+        <v>3347</v>
+      </c>
+      <c r="K1813">
+        <v>695336</v>
+      </c>
+      <c r="L1813" t="s">
+        <v>3347</v>
+      </c>
+      <c r="M1813" t="s">
+        <v>3347</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating daily files for Sept 26
</commit_message>
<xml_diff>
--- a/assets/My_Hitter_Listing.xlsx
+++ b/assets/My_Hitter_Listing.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28112"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Python\dash\dashenv\github\matchup\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAFBAAC3-74F0-42F7-BF5A-D6B45A200DC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99A5AB6E-09A0-4E1D-A17D-956538318D8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21146" uniqueCount="3350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21234" uniqueCount="3357">
   <si>
     <t>mlb_name</t>
   </si>
@@ -10079,10 +10079,31 @@
     <t>Thomas Saggese</t>
   </si>
   <si>
+    <t>Luisangel Acuna</t>
+  </si>
+  <si>
+    <t>Nick Yorke</t>
+  </si>
+  <si>
+    <t>Eric Wagaman</t>
+  </si>
+  <si>
+    <t>Gustavo Campero</t>
+  </si>
+  <si>
+    <t>Hunter Feduccia</t>
+  </si>
+  <si>
+    <t>Brandon Lockridge</t>
+  </si>
+  <si>
+    <t>Luis Vazquez</t>
+  </si>
+  <si>
+    <t>Dustin Harris</t>
+  </si>
+  <si>
     <t>sa123</t>
-  </si>
-  <si>
-    <t>Luisangel Acuna</t>
   </si>
 </sst>
 </file>
@@ -10479,11 +10500,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:M1814"/>
+  <dimension ref="A1:M1822"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1599" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K1612" sqref="K1612"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1798" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E1823" sqref="E1823"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -37858,10 +37879,10 @@
         <v>451</v>
       </c>
       <c r="B708" t="s">
-        <v>1428</v>
+        <v>1406</v>
       </c>
       <c r="C708" t="s">
-        <v>1458</v>
+        <v>1435</v>
       </c>
       <c r="D708" t="s">
         <v>1463</v>
@@ -77435,10 +77456,10 @@
         <v>3249</v>
       </c>
       <c r="B1725" t="s">
-        <v>1432</v>
+        <v>1429</v>
       </c>
       <c r="C1725" t="s">
-        <v>1462</v>
+        <v>1459</v>
       </c>
       <c r="D1725" t="s">
         <v>1465</v>
@@ -81054,7 +81075,7 @@
     </row>
     <row r="1814" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1814" t="s">
-        <v>3349</v>
+        <v>3348</v>
       </c>
       <c r="B1814" t="s">
         <v>1413</v>
@@ -81065,32 +81086,360 @@
       <c r="D1814" t="s">
         <v>1463</v>
       </c>
-      <c r="E1814" t="s">
+      <c r="E1814">
+        <v>26548</v>
+      </c>
+      <c r="F1814" t="s">
         <v>3348</v>
       </c>
-      <c r="F1814" t="s">
-        <v>3349</v>
-      </c>
       <c r="G1814" t="s">
-        <v>2760</v>
+        <v>1399</v>
       </c>
       <c r="H1814" t="s">
-        <v>3349</v>
+        <v>3348</v>
       </c>
       <c r="I1814" t="s">
-        <v>3349</v>
+        <v>3348</v>
       </c>
       <c r="J1814" t="s">
-        <v>3349</v>
+        <v>3348</v>
       </c>
       <c r="K1814">
         <v>682668</v>
       </c>
       <c r="L1814" t="s">
+        <v>3348</v>
+      </c>
+      <c r="M1814" t="s">
+        <v>3348</v>
+      </c>
+    </row>
+    <row r="1815" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1815" t="s">
         <v>3349</v>
       </c>
-      <c r="M1814" t="s">
+      <c r="B1815" t="s">
+        <v>1412</v>
+      </c>
+      <c r="C1815" t="s">
+        <v>1441</v>
+      </c>
+      <c r="D1815" t="s">
+        <v>1463</v>
+      </c>
+      <c r="E1815">
+        <v>27504</v>
+      </c>
+      <c r="F1815" t="s">
         <v>3349</v>
+      </c>
+      <c r="G1815" t="s">
+        <v>1401</v>
+      </c>
+      <c r="H1815" t="s">
+        <v>3349</v>
+      </c>
+      <c r="I1815" t="s">
+        <v>3349</v>
+      </c>
+      <c r="J1815" t="s">
+        <v>3349</v>
+      </c>
+      <c r="K1815">
+        <v>694377</v>
+      </c>
+      <c r="L1815" t="s">
+        <v>3349</v>
+      </c>
+      <c r="M1815" t="s">
+        <v>3349</v>
+      </c>
+    </row>
+    <row r="1816" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1816" t="s">
+        <v>3350</v>
+      </c>
+      <c r="B1816" t="s">
+        <v>1404</v>
+      </c>
+      <c r="C1816" t="s">
+        <v>1433</v>
+      </c>
+      <c r="D1816" t="s">
+        <v>1463</v>
+      </c>
+      <c r="E1816">
+        <v>23395</v>
+      </c>
+      <c r="F1816" t="s">
+        <v>3350</v>
+      </c>
+      <c r="G1816" t="s">
+        <v>1400</v>
+      </c>
+      <c r="H1816" t="s">
+        <v>3350</v>
+      </c>
+      <c r="I1816" t="s">
+        <v>3350</v>
+      </c>
+      <c r="J1816" t="s">
+        <v>3350</v>
+      </c>
+      <c r="K1816">
+        <v>676572</v>
+      </c>
+      <c r="L1816" t="s">
+        <v>3350</v>
+      </c>
+      <c r="M1816" t="s">
+        <v>3350</v>
+      </c>
+    </row>
+    <row r="1817" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1817" t="s">
+        <v>3351</v>
+      </c>
+      <c r="B1817" t="s">
+        <v>1404</v>
+      </c>
+      <c r="C1817" t="s">
+        <v>1433</v>
+      </c>
+      <c r="D1817" t="s">
+        <v>1465</v>
+      </c>
+      <c r="E1817">
+        <v>22707</v>
+      </c>
+      <c r="F1817" t="s">
+        <v>3351</v>
+      </c>
+      <c r="G1817" t="s">
+        <v>1398</v>
+      </c>
+      <c r="H1817" t="s">
+        <v>3351</v>
+      </c>
+      <c r="I1817" t="s">
+        <v>3351</v>
+      </c>
+      <c r="J1817" t="s">
+        <v>3351</v>
+      </c>
+      <c r="K1817">
+        <v>672569</v>
+      </c>
+      <c r="L1817" t="s">
+        <v>3351</v>
+      </c>
+      <c r="M1817" t="s">
+        <v>3351</v>
+      </c>
+    </row>
+    <row r="1818" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1818" t="s">
+        <v>2838</v>
+      </c>
+      <c r="B1818" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C1818" t="s">
+        <v>1450</v>
+      </c>
+      <c r="D1818" t="s">
+        <v>1464</v>
+      </c>
+      <c r="E1818">
+        <v>19314</v>
+      </c>
+      <c r="F1818" t="s">
+        <v>2838</v>
+      </c>
+      <c r="G1818" t="s">
+        <v>2760</v>
+      </c>
+      <c r="H1818" t="s">
+        <v>2838</v>
+      </c>
+      <c r="I1818" t="s">
+        <v>2838</v>
+      </c>
+      <c r="J1818" t="s">
+        <v>2838</v>
+      </c>
+      <c r="K1818">
+        <v>622268</v>
+      </c>
+      <c r="L1818" t="s">
+        <v>2838</v>
+      </c>
+      <c r="M1818" t="s">
+        <v>2838</v>
+      </c>
+    </row>
+    <row r="1819" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1819" t="s">
+        <v>3352</v>
+      </c>
+      <c r="B1819" t="s">
+        <v>1410</v>
+      </c>
+      <c r="C1819" t="s">
+        <v>1439</v>
+      </c>
+      <c r="D1819" t="s">
+        <v>1464</v>
+      </c>
+      <c r="E1819">
+        <v>23372</v>
+      </c>
+      <c r="F1819" t="s">
+        <v>3352</v>
+      </c>
+      <c r="G1819" t="s">
+        <v>1397</v>
+      </c>
+      <c r="H1819" t="s">
+        <v>3352</v>
+      </c>
+      <c r="I1819" t="s">
+        <v>3352</v>
+      </c>
+      <c r="J1819" t="s">
+        <v>3352</v>
+      </c>
+      <c r="K1819">
+        <v>676439</v>
+      </c>
+      <c r="L1819" t="s">
+        <v>3352</v>
+      </c>
+      <c r="M1819" t="s">
+        <v>3352</v>
+      </c>
+    </row>
+    <row r="1820" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1820" t="s">
+        <v>3353</v>
+      </c>
+      <c r="B1820" t="s">
+        <v>1406</v>
+      </c>
+      <c r="C1820" t="s">
+        <v>1435</v>
+      </c>
+      <c r="D1820" t="s">
+        <v>1463</v>
+      </c>
+      <c r="E1820">
+        <v>21496</v>
+      </c>
+      <c r="F1820" t="s">
+        <v>3353</v>
+      </c>
+      <c r="G1820" t="s">
+        <v>1398</v>
+      </c>
+      <c r="H1820" t="s">
+        <v>3353</v>
+      </c>
+      <c r="I1820" t="s">
+        <v>3353</v>
+      </c>
+      <c r="J1820" t="s">
+        <v>3353</v>
+      </c>
+      <c r="K1820">
+        <v>663604</v>
+      </c>
+      <c r="L1820" t="s">
+        <v>3353</v>
+      </c>
+      <c r="M1820" t="s">
+        <v>3353</v>
+      </c>
+    </row>
+    <row r="1821" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1821" t="s">
+        <v>3354</v>
+      </c>
+      <c r="B1821" t="s">
+        <v>1417</v>
+      </c>
+      <c r="C1821" t="s">
+        <v>1447</v>
+      </c>
+      <c r="D1821" t="s">
+        <v>1463</v>
+      </c>
+      <c r="E1821">
+        <v>23442</v>
+      </c>
+      <c r="F1821" t="s">
+        <v>3354</v>
+      </c>
+      <c r="G1821" t="s">
+        <v>2769</v>
+      </c>
+      <c r="H1821" t="s">
+        <v>3354</v>
+      </c>
+      <c r="I1821" t="s">
+        <v>3354</v>
+      </c>
+      <c r="J1821" t="s">
+        <v>3354</v>
+      </c>
+      <c r="K1821">
+        <v>676679</v>
+      </c>
+      <c r="L1821" t="s">
+        <v>3354</v>
+      </c>
+      <c r="M1821" t="s">
+        <v>3354</v>
+      </c>
+    </row>
+    <row r="1822" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1822" t="s">
+        <v>3355</v>
+      </c>
+      <c r="B1822" t="s">
+        <v>1407</v>
+      </c>
+      <c r="C1822" t="s">
+        <v>1436</v>
+      </c>
+      <c r="D1822" t="s">
+        <v>1464</v>
+      </c>
+      <c r="E1822" t="s">
+        <v>3356</v>
+      </c>
+      <c r="F1822" t="s">
+        <v>3355</v>
+      </c>
+      <c r="G1822" t="s">
+        <v>2768</v>
+      </c>
+      <c r="H1822" t="s">
+        <v>3355</v>
+      </c>
+      <c r="I1822" t="s">
+        <v>3355</v>
+      </c>
+      <c r="J1822" t="s">
+        <v>3355</v>
+      </c>
+      <c r="K1822">
+        <v>687957</v>
+      </c>
+      <c r="L1822" t="s">
+        <v>3355</v>
+      </c>
+      <c r="M1822" t="s">
+        <v>3355</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating daily files for Sept 27
</commit_message>
<xml_diff>
--- a/assets/My_Hitter_Listing.xlsx
+++ b/assets/My_Hitter_Listing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Python\dash\dashenv\github\matchup\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99A5AB6E-09A0-4E1D-A17D-956538318D8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59419B38-7332-48FA-BD77-97449F79FE86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21234" uniqueCount="3357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21245" uniqueCount="3358">
   <si>
     <t>mlb_name</t>
   </si>
@@ -10104,6 +10104,9 @@
   </si>
   <si>
     <t>sa123</t>
+  </si>
+  <si>
+    <t>Kevin Alcantara</t>
   </si>
 </sst>
 </file>
@@ -10500,11 +10503,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:M1822"/>
+  <dimension ref="A1:M1823"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1798" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1823" sqref="E1823"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1799" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K1824" sqref="K1824"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -81442,6 +81445,47 @@
         <v>3355</v>
       </c>
     </row>
+    <row r="1823" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1823" t="s">
+        <v>3357</v>
+      </c>
+      <c r="B1823" t="s">
+        <v>1417</v>
+      </c>
+      <c r="C1823" t="s">
+        <v>1447</v>
+      </c>
+      <c r="D1823" t="s">
+        <v>1463</v>
+      </c>
+      <c r="E1823">
+        <v>25971</v>
+      </c>
+      <c r="F1823" t="s">
+        <v>3357</v>
+      </c>
+      <c r="G1823" t="s">
+        <v>1398</v>
+      </c>
+      <c r="H1823" t="s">
+        <v>3357</v>
+      </c>
+      <c r="I1823" t="s">
+        <v>3357</v>
+      </c>
+      <c r="J1823" t="s">
+        <v>3357</v>
+      </c>
+      <c r="K1823">
+        <v>682634</v>
+      </c>
+      <c r="L1823" t="s">
+        <v>3357</v>
+      </c>
+      <c r="M1823" t="s">
+        <v>3357</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I1395">
     <sortCondition ref="A2:A1395"/>

</xml_diff>

<commit_message>
Update daily files April 25
</commit_message>
<xml_diff>
--- a/assets/My_Hitter_Listing.xlsx
+++ b/assets/My_Hitter_Listing.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28817"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shawn\Python\dash\dashenv\github\matchup\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E34428FA-FEF5-4873-9B80-FF421BE3A26F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A3A9CD6-0AA4-4C39-A2C1-30501C875361}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21802" uniqueCount="2147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21822" uniqueCount="2149">
   <si>
     <t>mlb_name</t>
   </si>
@@ -6479,6 +6479,12 @@
   </si>
   <si>
     <t>Chandler Simpson</t>
+  </si>
+  <si>
+    <t>Tirso Ornelas</t>
+  </si>
+  <si>
+    <t>Nick Kurtz</t>
   </si>
 </sst>
 </file>
@@ -6861,8 +6867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N1863"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1786" workbookViewId="0">
-      <selection activeCell="E1812" sqref="E1812"/>
+    <sheetView tabSelected="1" topLeftCell="A1788" workbookViewId="0">
+      <selection activeCell="K1814" sqref="K1814"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -84463,23 +84469,95 @@
       </c>
     </row>
     <row r="1812" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C1812" t="e">
+      <c r="A1812" t="s">
+        <v>2147</v>
+      </c>
+      <c r="B1812" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1812" t="str">
         <f>VLOOKUP(B1812,Teams!$A:$B,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N1812" t="e">
+        <v>San Diego Padres</v>
+      </c>
+      <c r="D1812" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1812">
+        <v>22566</v>
+      </c>
+      <c r="F1812" t="s">
+        <v>2147</v>
+      </c>
+      <c r="G1812" t="s">
+        <v>238</v>
+      </c>
+      <c r="H1812" t="s">
+        <v>2147</v>
+      </c>
+      <c r="I1812" t="s">
+        <v>2147</v>
+      </c>
+      <c r="J1812" t="s">
+        <v>2147</v>
+      </c>
+      <c r="K1812">
+        <v>672359</v>
+      </c>
+      <c r="L1812" t="s">
+        <v>2147</v>
+      </c>
+      <c r="M1812" t="s">
+        <v>2147</v>
+      </c>
+      <c r="N1812" t="str">
         <f>VLOOKUP(B1812,Teams!A:C,3,FALSE)</f>
-        <v>#N/A</v>
+        <v>San Diego</v>
       </c>
     </row>
     <row r="1813" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C1813" t="e">
+      <c r="A1813" t="s">
+        <v>2148</v>
+      </c>
+      <c r="B1813" t="s">
+        <v>156</v>
+      </c>
+      <c r="C1813" t="str">
         <f>VLOOKUP(B1813,Teams!$A:$B,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N1813" t="e">
+        <v>ATH</v>
+      </c>
+      <c r="D1813" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1813">
+        <v>35110</v>
+      </c>
+      <c r="F1813" t="s">
+        <v>2148</v>
+      </c>
+      <c r="G1813" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1813" t="s">
+        <v>2148</v>
+      </c>
+      <c r="I1813" t="s">
+        <v>2148</v>
+      </c>
+      <c r="J1813" t="s">
+        <v>2148</v>
+      </c>
+      <c r="K1813">
+        <v>701762</v>
+      </c>
+      <c r="L1813" t="s">
+        <v>2148</v>
+      </c>
+      <c r="M1813" t="s">
+        <v>2148</v>
+      </c>
+      <c r="N1813" t="str">
         <f>VLOOKUP(B1813,Teams!A:C,3,FALSE)</f>
-        <v>#N/A</v>
+        <v>ATH</v>
       </c>
     </row>
     <row r="1814" spans="1:14" x14ac:dyDescent="0.3">

</xml_diff>